<commit_message>
abbreviations and population data is not read in to be passed to the country
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="195">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -459,9 +459,6 @@
   </si>
   <si>
     <t xml:space="preserve">Skip years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2009, 2010</t>
   </si>
   <si>
     <t xml:space="preserve">Years that are sorted out before further data processing due to large deviations from the pattern of historical data.</t>
@@ -808,7 +805,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -857,23 +854,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps107.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps108.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps109.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps110.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps111.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps112.xml><?xml version="1.0" encoding="utf-8"?>
@@ -893,7 +890,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps116.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps117.xml><?xml version="1.0" encoding="utf-8"?>
@@ -901,7 +898,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps118.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps119.xml><?xml version="1.0" encoding="utf-8"?>
@@ -913,35 +910,35 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps126.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps128.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1077,7 +1074,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps30.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1121,7 +1118,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1165,7 +1162,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7565,8 +7562,8 @@
         <v>11</v>
       </c>
       <c r="C4" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>12</v>
@@ -7580,8 +7577,8 @@
         <v>13</v>
       </c>
       <c r="C5" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>14</v>
@@ -7595,8 +7592,8 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>16</v>
@@ -10682,7 +10679,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10807,11 +10804,11 @@
       <c r="B8" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>136</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>2009</v>
@@ -10819,7 +10816,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>6</v>
@@ -10828,7 +10825,7 @@
         <v>2019</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>2019</v>
@@ -10958,8 +10955,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10978,39 +10975,39 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>146</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="12" t="b">
@@ -11020,606 +11017,591 @@
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13" t="n">
+      <c r="J2" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="12" t="b">
+      <c r="C4" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" s="12" t="n">
+        <v>60</v>
+      </c>
+      <c r="J5" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="H11" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="J11" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="H12" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="J12" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="H13" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="J13" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="H14" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="J14" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="J15" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">D11</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">D12</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">D13</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="12" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">D14</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">D15</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="13" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="12" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H5" s="13" t="n">
-        <v>60</v>
-      </c>
-      <c r="J5" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="12" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H11" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="J11" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12" s="12" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H12" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="J12" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13" s="12" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H13" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="J13" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14" s="12" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H14" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="J14" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15" s="12" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H15" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="J15" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <f aca="false">D11</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="13" t="n">
-        <v>-0.23</v>
-      </c>
-      <c r="F16" s="9" t="n">
-        <f aca="false">100-F11</f>
-        <v>95</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C17" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <f aca="false">D12</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="9" t="n">
-        <f aca="false">100-F12</f>
-        <v>100</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C18" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <f aca="false">D13</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="13" t="n">
-        <v>-0.27</v>
-      </c>
-      <c r="F18" s="9" t="n">
-        <f aca="false">100-F13</f>
-        <v>100</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <f aca="false">D14</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9" t="n">
-        <f aca="false">100-F14</f>
-        <v>100</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C20" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <f aca="false">D15</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9" t="n">
-        <f aca="false">100-F15</f>
-        <v>100</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="C22" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H22" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="13" t="n">
+      <c r="J22" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="C23" s="12" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>170</v>
+      </c>
+      <c r="C23" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.33</v>
       </c>
-      <c r="E23" s="13" t="n">
+      <c r="E23" s="12" t="n">
         <v>0.33</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="13" t="n">
+      <c r="J23" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>173</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="4" t="n">
@@ -11632,7 +11614,7 @@
         <v>6</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H24" s="14" t="s">
         <v>6</v>
@@ -12200,7 +12182,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>123</v>
@@ -12211,13 +12193,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.45</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.45</v>
@@ -12225,13 +12207,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.83115</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.83115</v>
@@ -12239,13 +12221,13 @@
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
@@ -12253,13 +12235,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.35</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0.35</v>
@@ -12319,24 +12301,24 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>185</v>
-      </c>
       <c r="E2" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>6</v>
@@ -12345,7 +12327,7 @@
         <v>123</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>123</v>
@@ -12353,9 +12335,9 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="7" t="b">
+        <v>187</v>
+      </c>
+      <c r="C4" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12365,7 +12347,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
@@ -12374,7 +12356,7 @@
         <v>2018</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>2018</v>
@@ -12469,7 +12451,7 @@
       <c r="A2" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="7" t="b">
+      <c r="C2" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12479,14 +12461,14 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>25</v>
@@ -12494,18 +12476,18 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
@@ -12514,7 +12496,7 @@
         <v>2019</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>2019</v>
@@ -12522,7 +12504,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>6</v>
@@ -12531,7 +12513,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.5</v>
@@ -12620,17 +12602,17 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="12" t="b">
+      <c r="C2" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12642,67 +12624,67 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="12" t="b">
+      <c r="C4" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="12" t="b">
+      <c r="C5" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="12" t="b">
+      <c r="C6" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="12" t="b">
+      <c r="C7" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="12" t="b">
+      <c r="C8" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="12" t="b">
+      <c r="C9" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="12" t="b">
+      <c r="C10" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="12" t="b">
+      <c r="C11" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="12" t="b">
+      <c r="C12" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="12" t="b">
+      <c r="C13" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="12" t="b">
+      <c r="C14" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
input initialization finished for now
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -801,7 +801,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10679,7 +10679,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10955,7 +10955,7 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -12618,7 +12618,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="12" t="b">
+      <c r="C3" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
basic predictions work now.. i think
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" state="visible" r:id="rId2"/>
@@ -646,9 +646,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -752,7 +753,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -761,11 +762,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -773,7 +778,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -781,7 +786,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,11 +806,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,47 +859,47 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps106.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps107.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps108.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps109.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps110.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps111.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps112.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps113.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps114.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps115.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps116.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps117.xml><?xml version="1.0" encoding="utf-8"?>
@@ -898,11 +907,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps118.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -910,31 +919,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps126.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps128.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1386,13 +1395,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>28080</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1430,13 +1439,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>28080</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1474,13 +1483,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>27720</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1518,13 +1527,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>27720</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1562,13 +1571,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>27720</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1606,13 +1615,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>27720</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1650,13 +1659,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>28080</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1694,13 +1703,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>27720</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1738,13 +1747,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>6480</xdr:rowOff>
+          <xdr:rowOff>21600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1793,7 +1802,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>-309960</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>12960</xdr:rowOff>
+          <xdr:rowOff>28440</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -2766,7 +2775,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>-82800</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -6593,13 +6602,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>453600</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>15120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-612360</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>-69840</xdr:rowOff>
+          <xdr:rowOff>-54720</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -6648,7 +6657,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>6840</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>19080</xdr:rowOff>
+          <xdr:rowOff>34200</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -6741,7 +6750,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>-501480</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>12600</xdr:rowOff>
+          <xdr:rowOff>28080</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -7312,13 +7321,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>1527480</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>114480</xdr:rowOff>
+          <xdr:rowOff>129600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>429840</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>19080</xdr:rowOff>
+          <xdr:rowOff>34200</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -7525,20 +7534,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>2018</v>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>2050</v>
       </c>
     </row>
@@ -7546,14 +7555,14 @@
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="b">
+      <c r="C3" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7561,14 +7570,14 @@
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="b">
+      <c r="C4" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7576,14 +7585,14 @@
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="b">
+      <c r="C5" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7591,14 +7600,14 @@
       <c r="A6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="b">
+      <c r="C6" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7606,14 +7615,14 @@
       <c r="A7" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="b">
+      <c r="C7" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7621,14 +7630,14 @@
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="b">
+      <c r="C8" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7636,29 +7645,29 @@
       <c r="A9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="b">
+      <c r="C9" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" s="4" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+    <row r="10" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5" t="b">
+      <c r="C10" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -7669,13 +7678,13 @@
       <c r="B11" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="3" t="n">
         <v>2016</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="3" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -7683,14 +7692,14 @@
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="7" t="b">
+      <c r="C12" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7722,13 +7731,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>28080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7744,13 +7753,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>28080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7766,13 +7775,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>27720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7788,13 +7797,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>27720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7810,13 +7819,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>27720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7832,13 +7841,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>27720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7854,13 +7863,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>28080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7876,13 +7885,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>27720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7898,13 +7907,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>6480</xdr:rowOff>
+                    <xdr:rowOff>21600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7938,7 +7947,7 @@
       <c r="A1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -7947,13 +7956,13 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="7" t="b">
+      <c r="C2" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7962,7 +7971,7 @@
       <c r="A3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="7" t="b">
+      <c r="C3" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7971,7 +7980,7 @@
       <c r="A4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="7" t="b">
+      <c r="C4" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7980,7 +7989,7 @@
       <c r="A5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="7" t="b">
+      <c r="C5" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7989,7 +7998,7 @@
       <c r="A6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="7" t="b">
+      <c r="C6" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7998,7 +8007,7 @@
       <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="7" t="b">
+      <c r="C7" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8007,7 +8016,7 @@
       <c r="A8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="7" t="b">
+      <c r="C8" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8016,7 +8025,7 @@
       <c r="A9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="7" t="b">
+      <c r="C9" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8025,7 +8034,7 @@
       <c r="A10" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="7" t="b">
+      <c r="C10" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8034,7 +8043,7 @@
       <c r="A11" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="7" t="b">
+      <c r="C11" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8043,7 +8052,7 @@
       <c r="A12" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="7" t="b">
+      <c r="C12" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8052,7 +8061,7 @@
       <c r="A13" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="7" t="b">
+      <c r="C13" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8061,7 +8070,7 @@
       <c r="A14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="7" t="b">
+      <c r="C14" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8070,7 +8079,7 @@
       <c r="A15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="7" t="b">
+      <c r="C15" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8079,7 +8088,7 @@
       <c r="A16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="7" t="b">
+      <c r="C16" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8088,7 +8097,7 @@
       <c r="A17" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="7" t="b">
+      <c r="C17" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8097,7 +8106,7 @@
       <c r="A18" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="7" t="b">
+      <c r="C18" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8106,7 +8115,7 @@
       <c r="A19" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="7" t="b">
+      <c r="C19" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8115,7 +8124,7 @@
       <c r="A20" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="7" t="b">
+      <c r="C20" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8124,7 +8133,7 @@
       <c r="A21" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="7" t="b">
+      <c r="C21" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8133,7 +8142,7 @@
       <c r="A22" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="7" t="b">
+      <c r="C22" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8142,7 +8151,7 @@
       <c r="A23" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="7" t="b">
+      <c r="C23" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8151,7 +8160,7 @@
       <c r="A24" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="7" t="b">
+      <c r="C24" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8160,7 +8169,7 @@
       <c r="A25" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="7" t="b">
+      <c r="C25" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8169,7 +8178,7 @@
       <c r="A26" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="7" t="b">
+      <c r="C26" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8178,7 +8187,7 @@
       <c r="A27" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="7" t="b">
+      <c r="C27" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8187,7 +8196,7 @@
       <c r="A28" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="7" t="b">
+      <c r="C28" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8196,7 +8205,7 @@
       <c r="A29" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="7" t="b">
+      <c r="C29" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8205,7 +8214,7 @@
       <c r="A30" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="7" t="b">
+      <c r="C30" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8214,7 +8223,7 @@
       <c r="A31" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="7" t="b">
+      <c r="C31" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8223,7 +8232,7 @@
       <c r="A32" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="7" t="b">
+      <c r="C32" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8232,7 +8241,7 @@
       <c r="A33" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="7" t="b">
+      <c r="C33" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8241,7 +8250,7 @@
       <c r="A34" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="7" t="b">
+      <c r="C34" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8250,7 +8259,7 @@
       <c r="A35" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="7" t="b">
+      <c r="C35" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8259,7 +8268,7 @@
       <c r="A36" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="7" t="b">
+      <c r="C36" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8271,7 +8280,7 @@
       <c r="A37" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="7" t="b">
+      <c r="C37" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8283,7 +8292,7 @@
       <c r="A38" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="7" t="b">
+      <c r="C38" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8292,7 +8301,7 @@
       <c r="A39" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="7" t="b">
+      <c r="C39" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8301,7 +8310,7 @@
       <c r="A40" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="7" t="b">
+      <c r="C40" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8310,7 +8319,7 @@
       <c r="A41" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="7" t="b">
+      <c r="C41" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8319,7 +8328,7 @@
       <c r="A42" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="7" t="b">
+      <c r="C42" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8328,7 +8337,7 @@
       <c r="A43" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="7" t="b">
+      <c r="C43" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8337,7 +8346,7 @@
       <c r="A44" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="7" t="b">
+      <c r="C44" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8346,7 +8355,7 @@
       <c r="A45" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="7" t="b">
+      <c r="C45" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8355,7 +8364,7 @@
       <c r="A46" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="7" t="b">
+      <c r="C46" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8364,7 +8373,7 @@
       <c r="A47" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="7" t="b">
+      <c r="C47" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8373,7 +8382,7 @@
       <c r="A48" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="7" t="b">
+      <c r="C48" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8382,7 +8391,7 @@
       <c r="A49" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="7" t="b">
+      <c r="C49" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8391,7 +8400,7 @@
       <c r="A50" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="7" t="b">
+      <c r="C50" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8400,7 +8409,7 @@
       <c r="A51" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="7" t="b">
+      <c r="C51" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8409,7 +8418,7 @@
       <c r="A52" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="7" t="b">
+      <c r="C52" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8418,7 +8427,7 @@
       <c r="A53" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C53" s="7" t="b">
+      <c r="C53" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8427,7 +8436,7 @@
       <c r="A54" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="7" t="b">
+      <c r="C54" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8436,7 +8445,7 @@
       <c r="A55" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="7" t="b">
+      <c r="C55" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8445,7 +8454,7 @@
       <c r="A56" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="7" t="b">
+      <c r="C56" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8454,7 +8463,7 @@
       <c r="A57" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="7" t="b">
+      <c r="C57" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8463,7 +8472,7 @@
       <c r="A58" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="7" t="b">
+      <c r="C58" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8472,7 +8481,7 @@
       <c r="A59" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="7" t="b">
+      <c r="C59" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8481,7 +8490,7 @@
       <c r="A60" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="7" t="b">
+      <c r="C60" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8490,7 +8499,7 @@
       <c r="A61" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="7" t="b">
+      <c r="C61" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8499,7 +8508,7 @@
       <c r="A62" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="7" t="b">
+      <c r="C62" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8508,7 +8517,7 @@
       <c r="A63" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="7" t="b">
+      <c r="C63" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8517,7 +8526,7 @@
       <c r="A64" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="7" t="b">
+      <c r="C64" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8526,7 +8535,7 @@
       <c r="A65" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C65" s="7" t="b">
+      <c r="C65" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8535,7 +8544,7 @@
       <c r="A66" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="7" t="b">
+      <c r="C66" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8544,7 +8553,7 @@
       <c r="A67" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="7" t="b">
+      <c r="C67" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8553,7 +8562,7 @@
       <c r="A68" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C68" s="7" t="b">
+      <c r="C68" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8562,7 +8571,7 @@
       <c r="A69" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C69" s="7" t="b">
+      <c r="C69" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8571,7 +8580,7 @@
       <c r="A70" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="7" t="b">
+      <c r="C70" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8580,7 +8589,7 @@
       <c r="A71" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C71" s="7" t="b">
+      <c r="C71" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8589,7 +8598,7 @@
       <c r="A72" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C72" s="7" t="b">
+      <c r="C72" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8598,7 +8607,7 @@
       <c r="A73" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C73" s="7" t="b">
+      <c r="C73" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8607,7 +8616,7 @@
       <c r="A74" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="7" t="b">
+      <c r="C74" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8616,7 +8625,7 @@
       <c r="A75" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="C75" s="7" t="b">
+      <c r="C75" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8625,7 +8634,7 @@
       <c r="A76" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C76" s="7" t="b">
+      <c r="C76" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8634,7 +8643,7 @@
       <c r="A77" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="C77" s="7" t="b">
+      <c r="C77" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8643,7 +8652,7 @@
       <c r="A78" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="7" t="b">
+      <c r="C78" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8652,7 +8661,7 @@
       <c r="A79" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C79" s="7" t="b">
+      <c r="C79" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8661,7 +8670,7 @@
       <c r="A80" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C80" s="7" t="b">
+      <c r="C80" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8670,7 +8679,7 @@
       <c r="A81" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C81" s="7" t="b">
+      <c r="C81" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8679,7 +8688,7 @@
       <c r="A82" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C82" s="7" t="b">
+      <c r="C82" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8688,7 +8697,7 @@
       <c r="A83" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C83" s="7" t="b">
+      <c r="C83" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8697,7 +8706,7 @@
       <c r="A84" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C84" s="7" t="b">
+      <c r="C84" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8706,7 +8715,7 @@
       <c r="A85" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C85" s="7" t="b">
+      <c r="C85" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8715,7 +8724,7 @@
       <c r="A86" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="7" t="b">
+      <c r="C86" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8724,7 +8733,7 @@
       <c r="A87" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C87" s="7" t="b">
+      <c r="C87" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8733,7 +8742,7 @@
       <c r="A88" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C88" s="7" t="b">
+      <c r="C88" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8766,7 +8775,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>-82800</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10678,8 +10687,8 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10713,7 +10722,7 @@
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>123</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -10727,7 +10736,7 @@
       <c r="A3" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="7" t="b">
+      <c r="C3" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -10742,7 +10751,7 @@
       <c r="A4" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="7" t="b">
+      <c r="C4" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10757,7 +10766,7 @@
       <c r="A5" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="7" t="b">
+      <c r="C5" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10786,7 +10795,7 @@
       <c r="A7" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="7" t="b">
+      <c r="C7" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10863,13 +10872,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1527480</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>114480</xdr:rowOff>
+                    <xdr:rowOff>129600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>429840</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>19080</xdr:rowOff>
+                    <xdr:rowOff>34200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10955,8 +10964,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10980,28 +10989,28 @@
       <c r="B1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>143</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>142</v>
       </c>
     </row>
@@ -11010,26 +11019,25 @@
         <v>146</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="12" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C2" s="13" t="b">
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="12" t="n">
+      <c r="J2" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11039,25 +11047,24 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="12" t="n">
+      <c r="J3" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11066,25 +11073,24 @@
         <v>149</v>
       </c>
       <c r="C4" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="12" t="n">
+      <c r="J4" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11093,13 +11099,12 @@
         <v>150</v>
       </c>
       <c r="C5" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="0" t="n">
@@ -11108,10 +11113,10 @@
       <c r="G5" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="H5" s="12" t="n">
+      <c r="H5" s="14" t="n">
         <v>60</v>
       </c>
-      <c r="J5" s="12" t="n">
+      <c r="J5" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11120,25 +11125,24 @@
         <v>152</v>
       </c>
       <c r="C6" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="12" t="n">
+      <c r="J6" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11147,25 +11151,24 @@
         <v>153</v>
       </c>
       <c r="C7" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="12" t="n">
+      <c r="J7" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11174,25 +11177,24 @@
         <v>154</v>
       </c>
       <c r="C8" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="12" t="n">
+      <c r="J8" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11201,25 +11203,24 @@
         <v>155</v>
       </c>
       <c r="C9" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="12" t="n">
+      <c r="J9" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11228,25 +11229,24 @@
         <v>156</v>
       </c>
       <c r="C10" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="E10" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="12" t="n">
+      <c r="J10" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11255,13 +11255,12 @@
         <v>157</v>
       </c>
       <c r="C11" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="12" t="n">
+      <c r="E11" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
@@ -11270,10 +11269,10 @@
       <c r="G11" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="H11" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="J11" s="12" t="n">
+      <c r="J11" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11282,13 +11281,12 @@
         <v>159</v>
       </c>
       <c r="C12" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="12" t="n">
+      <c r="E12" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -11297,10 +11295,10 @@
       <c r="G12" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="H12" s="12" t="n">
+      <c r="H12" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="J12" s="12" t="n">
+      <c r="J12" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11309,13 +11307,12 @@
         <v>160</v>
       </c>
       <c r="C13" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="12" t="n">
+      <c r="E13" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="0" t="n">
@@ -11324,10 +11321,10 @@
       <c r="G13" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="H13" s="12" t="n">
+      <c r="H13" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="J13" s="12" t="n">
+      <c r="J13" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11336,13 +11333,12 @@
         <v>161</v>
       </c>
       <c r="C14" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="12" t="n">
+      <c r="E14" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
@@ -11351,10 +11347,10 @@
       <c r="G14" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="H14" s="12" t="n">
+      <c r="H14" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="J14" s="12" t="n">
+      <c r="J14" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11363,13 +11359,12 @@
         <v>162</v>
       </c>
       <c r="C15" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="12" t="n">
+      <c r="E15" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="0" t="n">
@@ -11378,10 +11373,10 @@
       <c r="G15" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="H15" s="12" t="n">
+      <c r="H15" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="J15" s="12" t="n">
+      <c r="J15" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11390,24 +11385,23 @@
         <v>163</v>
       </c>
       <c r="C16" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">D11</f>
         <v>0</v>
       </c>
-      <c r="E16" s="12" t="n">
+      <c r="E16" s="14" t="n">
         <v>-0.23</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="12" t="n">
+      <c r="J16" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11416,24 +11410,23 @@
         <v>164</v>
       </c>
       <c r="C17" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">D12</f>
         <v>0</v>
       </c>
-      <c r="E17" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="9"/>
+      <c r="E17" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10"/>
       <c r="G17" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="12" t="n">
+      <c r="J17" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11442,24 +11435,23 @@
         <v>165</v>
       </c>
       <c r="C18" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">D13</f>
         <v>0</v>
       </c>
-      <c r="E18" s="12" t="n">
+      <c r="E18" s="14" t="n">
         <v>-0.27</v>
       </c>
-      <c r="F18" s="9"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="12" t="n">
+      <c r="J18" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11468,24 +11460,23 @@
         <v>166</v>
       </c>
       <c r="C19" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">D14</f>
         <v>0</v>
       </c>
-      <c r="E19" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9"/>
+      <c r="E19" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10"/>
       <c r="G19" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="12" t="n">
+      <c r="J19" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11494,24 +11485,23 @@
         <v>167</v>
       </c>
       <c r="C20" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">D15</f>
         <v>0</v>
       </c>
-      <c r="E20" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9"/>
+      <c r="E20" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10"/>
       <c r="G20" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="12" t="n">
+      <c r="J20" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11520,25 +11510,24 @@
         <v>168</v>
       </c>
       <c r="C21" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="9" t="s">
+      <c r="E21" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J21" s="12" t="n">
+      <c r="J21" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11546,26 +11535,26 @@
       <c r="A22" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C22" s="13" t="b">
+      <c r="C22" s="15" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="9" t="s">
+      <c r="E22" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="12" t="n">
+      <c r="J22" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11574,53 +11563,52 @@
         <v>170</v>
       </c>
       <c r="C23" s="13" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.33</v>
       </c>
-      <c r="E23" s="12" t="n">
+      <c r="E23" s="14" t="n">
         <v>0.33</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="12" t="n">
+      <c r="J23" s="14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="4" t="n">
+      <c r="C24" s="16"/>
+      <c r="D24" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="E24" s="14" t="n">
+      <c r="E24" s="16" t="n">
         <v>0.7</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="14" t="n">
+      <c r="I24" s="5"/>
+      <c r="J24" s="16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11674,7 +11662,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>-309960</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>12960</xdr:rowOff>
+                    <xdr:rowOff>28440</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12184,7 +12172,7 @@
       <c r="A2" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>123</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -12226,7 +12214,7 @@
       <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>179</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -12306,7 +12294,7 @@
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>183</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -12323,10 +12311,10 @@
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>186</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -12337,7 +12325,7 @@
       <c r="A4" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="0" t="b">
+      <c r="C4" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12394,13 +12382,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>453600</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:rowOff>15120</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-612360</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>-69840</xdr:rowOff>
+                    <xdr:rowOff>-54720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12451,7 +12439,7 @@
       <c r="A2" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="0" t="b">
+      <c r="C2" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12463,7 +12451,7 @@
       <c r="A3" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="7" t="b">
+      <c r="C3" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12547,7 +12535,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>6840</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>19080</xdr:rowOff>
+                    <xdr:rowOff>34200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12607,84 +12595,84 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="13" t="b">
+      <c r="C2" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="13" t="b">
+      <c r="C3" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="13" t="b">
+      <c r="C4" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="13" t="b">
+      <c r="C5" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="13" t="b">
+      <c r="C6" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="13" t="b">
+      <c r="C7" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="13" t="b">
+      <c r="C8" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="13" t="b">
+      <c r="C9" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="13" t="b">
+      <c r="C10" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="13" t="b">
+      <c r="C11" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="13" t="b">
+      <c r="C12" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="13" t="b">
+      <c r="C13" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="13" t="b">
+      <c r="C14" s="15" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12717,7 +12705,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>-501480</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>12600</xdr:rowOff>
+                    <xdr:rowOff>28080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
completed product demand calculation in the most basic sense and now trying to replicate the reference data
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" state="visible" r:id="rId2"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="200">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -146,6 +146,12 @@
     <t xml:space="preserve">Graphical representation of results in the case all sectors are activated</t>
   </si>
   <si>
+    <t xml:space="preserve">Calculate final energy demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For calculation of the share of the industrial non-specified sector</t>
+  </si>
+  <si>
     <t xml:space="preserve">Country</t>
   </si>
   <si>
@@ -575,9 +581,6 @@
     <t xml:space="preserve">allways active</t>
   </si>
   <si>
-    <t xml:space="preserve">Forecast method for rest household consumption</t>
-  </si>
-  <si>
     <t xml:space="preserve">Predefined ratio of Q1 heat level (below 60°C)</t>
   </si>
   <si>
@@ -614,11 +617,22 @@
     <t xml:space="preserve">Method for modal split</t>
   </si>
   <si>
-    <t xml:space="preserve">If scenario selection = study values =&gt; method = Trend (interpolation of values is done). 
-If scenario selection = historical =&gt; method can be both Trend or Constant (trend development or last available value)</t>
+    <t xml:space="preserve">If scenario selection = historical =&gt; method can be both Trend or Constant (linear trend development or last available value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario selection for final energy demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario selection for final energy demand calaculation - electricity and hydrogen vehicles shares based on reference case or user inputs</t>
   </si>
   <si>
     <t xml:space="preserve">Calculation for rest subsector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario selection for final energy demand calaculation - electricity and hydrogen vehicles shares</t>
   </si>
   <si>
     <t xml:space="preserve">Reference year for industrial production</t>
@@ -646,10 +660,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -753,7 +766,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -762,15 +775,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -778,7 +787,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -786,7 +795,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -810,11 +819,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -838,204 +843,204 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$10" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps100.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps101.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$7" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps102.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_general!$C$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps103.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_general!$C$4" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps103.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps104.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_general!$C$3" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps105.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps106.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$2" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps106.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$5" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProps107.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps108.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$6" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps108.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps109.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$7" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps109.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$13" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps110.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps110.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps111.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$9" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps111.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps112.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$10" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps112.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$12" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProps113.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps114.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps115.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps116.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$15" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps117.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$21" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps117.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps118.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$22" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps118.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps119.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$23" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps120.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps121.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$16" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps122.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$19" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps123.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$20" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps124.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps125.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$17" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps126.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps127.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps129.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps13.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$2" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$16" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$19" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$20" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$18" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$17" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps126.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="IND_subsectors!$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps128.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps131.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$2" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps132.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="CTS!$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps134.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps135.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps136.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps137.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps138.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$7" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps139.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps14.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$3" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps130.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$2" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps131.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="CTS!$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps133.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps134.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps135.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps136.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$6" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps137.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$7" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps138.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps139.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps140.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$9" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps141.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps142.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps143.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$12" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps144.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$13" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps145.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$14" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps146.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$2" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps15.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$4" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps140.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$10" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps141.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps142.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$12" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps143.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$13" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps144.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$14" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps145.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="IND_food_unused!$C$2" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps16.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps17.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$6" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps18.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$7" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps19.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1043,175 +1048,175 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps21.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$10" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps22.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$11" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps23.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$12" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps24.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$13" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps25.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$14" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps26.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$15" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps27.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$16" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps28.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$17" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps29.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps30.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$19" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps31.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$20" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps32.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$21" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps33.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$22" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps34.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$23" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps35.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$24" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps36.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$25" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps37.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$26" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps38.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$27" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps39.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$28" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps40.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$29" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps41.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$30" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps42.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$31" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps43.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$32" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps44.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$34" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps45.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$35" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps46.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="Countries!$C$33" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps47.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$36" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps48.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$37" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps49.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$38" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps50.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$39" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="GeneralSettings!$C$6" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps51.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$40" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps52.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$41" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps53.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$42" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps54.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$43" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps55.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$44" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps56.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$45" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps57.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$46" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps58.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$47" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps59.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$54" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps59.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$52" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1219,43 +1224,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps60.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$52" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps61.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$51" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps62.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$55" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps63.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$56" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps64.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$57" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps65.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$58" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps66.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$59" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps67.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$60" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps68.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$50" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps69.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$49" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps69.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1263,43 +1268,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps70.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$62" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps71.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$61" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps72.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$63" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps73.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$64" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps74.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$65" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps75.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$66" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps76.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$67" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps77.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$68" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps78.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$69" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps79.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$70" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps79.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$71" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1307,43 +1312,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps80.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$71" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps81.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$72" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps82.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$73" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps83.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$74" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps84.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$75" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps85.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$76" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps86.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$77" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps87.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$78" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps88.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$79" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps89.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$80" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProps89.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$81" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProps9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1351,38 +1356,42 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProps90.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$81" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProps91.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$82" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps92.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$83" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps93.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$84" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps94.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$85" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps95.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$86" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps96.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$87" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps97.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$88" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps98.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$53" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProps98.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProps99.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" autoLine="false" print="true" fmlaLink="Countries!$C$48" lockText="1" noThreeD="1"/>
 </file>
 
@@ -1395,13 +1404,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>28080</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1439,13 +1448,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>15480</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>28080</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1483,13 +1492,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>15480</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>27720</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1527,13 +1536,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>27720</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1571,13 +1580,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>27720</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1615,13 +1624,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>27720</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1659,13 +1668,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>28080</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1703,13 +1712,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>27720</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1747,13 +1756,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>6480</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>15480</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>-818280</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>21600</xdr:rowOff>
+          <xdr:rowOff>6480</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -1784,10 +1793,235 @@
       </xdr:twoCellAnchor>
     </mc:Choice>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>6480</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>-818280</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>12600</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1010" name="Check Box 13" descr="Activate" hidden="0"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr anchor="ctr">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:p>
+              <a:r>
+                <a:t>Activate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing104.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing100.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1527480</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>114480</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>429840</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19080</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1001" name="Check Box 4" descr="Activate" hidden="0"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr anchor="ctr">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:p>
+              <a:r>
+                <a:t>Activate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>6480</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>114480</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>-789480</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19080</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1002" name="Check Box 5" descr="Activate" hidden="0"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr anchor="ctr">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:p>
+              <a:r>
+                <a:t>Activate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>6480</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>114480</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>-789480</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19080</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1003" name="Check Box 6" descr="Activate" hidden="0"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr anchor="ctr">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:p>
+              <a:r>
+                <a:t>Activate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>6480</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>114480</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>-789480</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>19080</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1004" name="Check Box 7" descr="Activate" hidden="0"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr anchor="ctr">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:p>
+              <a:r>
+                <a:t>Activate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing105.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -1802,7 +2036,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>-309960</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>28440</xdr:rowOff>
+          <xdr:rowOff>12960</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -2760,7 +2994,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -2775,7 +3009,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>-82800</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -6593,22 +6827,22 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing127.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing128.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>453600</xdr:colOff>
+          <xdr:colOff>654840</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>15120</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>-612360</xdr:colOff>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>-411120</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>-54720</xdr:rowOff>
+          <xdr:rowOff>-69840</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -6642,7 +6876,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing129.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing130.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -6657,7 +6891,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>6840</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>34200</xdr:rowOff>
+          <xdr:rowOff>19080</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -6735,7 +6969,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing132.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing133.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -6750,7 +6984,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>-501480</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>28080</xdr:rowOff>
+          <xdr:rowOff>12600</xdr:rowOff>
         </xdr:to>
         <xdr:sp>
           <xdr:nvSpPr>
@@ -7283,187 +7517,6 @@
         <xdr:sp>
           <xdr:nvSpPr>
             <xdr:cNvPr id="1013" name="Check Box 26" descr="Activate" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing99.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1527480</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>129600</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>429840</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>34200</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1001" name="Check Box 4" descr="Activate" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>6480</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>114480</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>-789480</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>19080</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1002" name="Check Box 5" descr="Activate" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>6480</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>114480</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>-789480</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>19080</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1003" name="Check Box 6" descr="Activate" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>6480</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>114480</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>-789480</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>19080</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1004" name="Check Box 7" descr="Activate" hidden="0"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -7498,10 +7551,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7534,20 +7587,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="b">
-        <v>1</v>
+      <c r="C2" s="2" t="n">
+        <v>2018</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="2" t="n">
         <v>2050</v>
       </c>
     </row>
@@ -7555,14 +7608,14 @@
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="b">
+      <c r="C3" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7570,14 +7623,14 @@
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7585,14 +7638,14 @@
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C5" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7600,14 +7653,14 @@
       <c r="A6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C6" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7615,14 +7668,14 @@
       <c r="A7" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="b">
+      <c r="C7" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7630,14 +7683,14 @@
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="b">
+      <c r="C8" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7645,29 +7698,29 @@
       <c r="A9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="b">
+      <c r="C9" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+    <row r="10" s="4" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6" t="b">
+      <c r="C10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -7678,13 +7731,13 @@
       <c r="B11" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="2" t="n">
         <v>2016</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="2" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -7692,15 +7745,30 @@
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8" t="b">
+      <c r="C12" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -7731,13 +7799,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>28080</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7753,13 +7821,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>15480</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>28080</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7775,13 +7843,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>15480</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>27720</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7797,13 +7865,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>27720</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7819,13 +7887,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>27720</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7841,13 +7909,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>27720</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7863,13 +7931,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>28080</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7885,13 +7953,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>27720</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7907,13 +7975,35 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>6480</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>15480</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>-818280</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>21600</xdr:rowOff>
+                    <xdr:rowOff>6480</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1010" r:id="rId12" name="Activate">
+              <controlPr defaultSize="0" locked="1" autoFill="0" autoLine="0" autoPict="0" print="true" altText="Check Box 13">
+                <anchor moveWithCells="true" sizeWithCells="false">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>6480</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>-818280</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7933,8 +8023,8 @@
   </sheetPr>
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7945,804 +8035,804 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="8" t="b">
+        <v>34</v>
+      </c>
+      <c r="C2" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="8" t="b">
+        <v>35</v>
+      </c>
+      <c r="C3" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="8" t="b">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="8" t="b">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="8" t="b">
+        <v>38</v>
+      </c>
+      <c r="C6" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="8" t="b">
+        <v>39</v>
+      </c>
+      <c r="C7" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="8" t="b">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="8" t="b">
+        <v>41</v>
+      </c>
+      <c r="C9" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="8" t="b">
+        <v>42</v>
+      </c>
+      <c r="C10" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="8" t="b">
+        <v>43</v>
+      </c>
+      <c r="C11" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="8" t="b">
+        <v>44</v>
+      </c>
+      <c r="C12" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="8" t="b">
+        <v>45</v>
+      </c>
+      <c r="C13" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="8" t="b">
+        <v>46</v>
+      </c>
+      <c r="C14" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="8" t="b">
+        <v>47</v>
+      </c>
+      <c r="C15" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="8" t="b">
+        <v>48</v>
+      </c>
+      <c r="C16" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="8" t="b">
+        <v>49</v>
+      </c>
+      <c r="C17" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="8" t="b">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="8" t="b">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="8" t="b">
+        <v>52</v>
+      </c>
+      <c r="C20" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="8" t="b">
+        <v>53</v>
+      </c>
+      <c r="C21" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="8" t="b">
+        <v>54</v>
+      </c>
+      <c r="C22" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="8" t="b">
+        <v>55</v>
+      </c>
+      <c r="C23" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="8" t="b">
+        <v>56</v>
+      </c>
+      <c r="C24" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="8" t="b">
+        <v>57</v>
+      </c>
+      <c r="C25" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="8" t="b">
+        <v>58</v>
+      </c>
+      <c r="C26" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="8" t="b">
+        <v>59</v>
+      </c>
+      <c r="C27" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="8" t="b">
+        <v>60</v>
+      </c>
+      <c r="C28" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="8" t="b">
+        <v>61</v>
+      </c>
+      <c r="C29" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="8" t="b">
+        <v>62</v>
+      </c>
+      <c r="C30" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="8" t="b">
+        <v>63</v>
+      </c>
+      <c r="C31" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="8" t="b">
+        <v>64</v>
+      </c>
+      <c r="C32" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="8" t="b">
+        <v>65</v>
+      </c>
+      <c r="C33" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="8" t="b">
+        <v>66</v>
+      </c>
+      <c r="C34" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="8" t="b">
+        <v>67</v>
+      </c>
+      <c r="C35" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="8" t="b">
+        <v>68</v>
+      </c>
+      <c r="C36" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="8" t="b">
+        <v>70</v>
+      </c>
+      <c r="C37" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="8" t="b">
+        <v>72</v>
+      </c>
+      <c r="C38" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="8" t="b">
+        <v>73</v>
+      </c>
+      <c r="C39" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="8" t="b">
+        <v>74</v>
+      </c>
+      <c r="C40" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="8" t="b">
+        <v>75</v>
+      </c>
+      <c r="C41" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="8" t="b">
+        <v>76</v>
+      </c>
+      <c r="C42" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="8" t="b">
+        <v>77</v>
+      </c>
+      <c r="C43" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="8" t="b">
+        <v>78</v>
+      </c>
+      <c r="C44" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="8" t="b">
+        <v>79</v>
+      </c>
+      <c r="C45" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="8" t="b">
+        <v>80</v>
+      </c>
+      <c r="C46" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="8" t="b">
+        <v>81</v>
+      </c>
+      <c r="C47" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="8" t="b">
+        <v>82</v>
+      </c>
+      <c r="C48" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="8" t="b">
+        <v>83</v>
+      </c>
+      <c r="C49" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" s="8" t="b">
+        <v>84</v>
+      </c>
+      <c r="C50" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="8" t="b">
+        <v>85</v>
+      </c>
+      <c r="C51" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C52" s="8" t="b">
+        <v>86</v>
+      </c>
+      <c r="C52" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C53" s="8" t="b">
+        <v>87</v>
+      </c>
+      <c r="C53" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="8" t="b">
+        <v>88</v>
+      </c>
+      <c r="C54" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" s="8" t="b">
+        <v>89</v>
+      </c>
+      <c r="C55" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" s="8" t="b">
+        <v>90</v>
+      </c>
+      <c r="C56" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" s="8" t="b">
+        <v>91</v>
+      </c>
+      <c r="C57" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="8" t="b">
+        <v>92</v>
+      </c>
+      <c r="C58" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" s="8" t="b">
+        <v>93</v>
+      </c>
+      <c r="C59" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C60" s="8" t="b">
+        <v>94</v>
+      </c>
+      <c r="C60" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="8" t="b">
+        <v>95</v>
+      </c>
+      <c r="C61" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="8" t="b">
+        <v>96</v>
+      </c>
+      <c r="C62" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="8" t="b">
+        <v>97</v>
+      </c>
+      <c r="C63" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="8" t="b">
+        <v>98</v>
+      </c>
+      <c r="C64" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="8" t="b">
+        <v>99</v>
+      </c>
+      <c r="C65" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" s="8" t="b">
+        <v>100</v>
+      </c>
+      <c r="C66" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="8" t="b">
+        <v>101</v>
+      </c>
+      <c r="C67" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="8" t="b">
+        <v>102</v>
+      </c>
+      <c r="C68" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" s="8" t="b">
+        <v>103</v>
+      </c>
+      <c r="C69" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C70" s="8" t="b">
+        <v>104</v>
+      </c>
+      <c r="C70" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C71" s="8" t="b">
+        <v>105</v>
+      </c>
+      <c r="C71" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="C72" s="8" t="b">
+        <v>106</v>
+      </c>
+      <c r="C72" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C73" s="8" t="b">
+        <v>107</v>
+      </c>
+      <c r="C73" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C74" s="8" t="b">
+        <v>108</v>
+      </c>
+      <c r="C74" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C75" s="8" t="b">
+        <v>109</v>
+      </c>
+      <c r="C75" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C76" s="8" t="b">
+        <v>110</v>
+      </c>
+      <c r="C76" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" s="8" t="b">
+        <v>111</v>
+      </c>
+      <c r="C77" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C78" s="8" t="b">
+        <v>112</v>
+      </c>
+      <c r="C78" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C79" s="8" t="b">
+        <v>113</v>
+      </c>
+      <c r="C79" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C80" s="8" t="b">
+        <v>114</v>
+      </c>
+      <c r="C80" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C81" s="8" t="b">
+        <v>115</v>
+      </c>
+      <c r="C81" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C82" s="8" t="b">
+        <v>116</v>
+      </c>
+      <c r="C82" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C83" s="8" t="b">
+        <v>117</v>
+      </c>
+      <c r="C83" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C84" s="8" t="b">
+        <v>118</v>
+      </c>
+      <c r="C84" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C85" s="8" t="b">
+        <v>119</v>
+      </c>
+      <c r="C85" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C86" s="8" t="b">
+        <v>120</v>
+      </c>
+      <c r="C86" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C87" s="8" t="b">
+        <v>121</v>
+      </c>
+      <c r="C87" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C88" s="8" t="b">
+        <v>122</v>
+      </c>
+      <c r="C88" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8775,7 +8865,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>-82800</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10687,8 +10777,8 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10712,36 +10802,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>123</v>
+      <c r="C2" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="8" t="b">
+        <v>127</v>
+      </c>
+      <c r="C3" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>25</v>
@@ -10749,14 +10839,14 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="8" t="b">
+        <v>129</v>
+      </c>
+      <c r="C4" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>10</v>
@@ -10764,9 +10854,9 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="8" t="b">
+        <v>131</v>
+      </c>
+      <c r="C5" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10776,7 +10866,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>6</v>
@@ -10785,7 +10875,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
@@ -10793,14 +10883,14 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="8" t="b">
+        <v>134</v>
+      </c>
+      <c r="C7" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>10</v>
@@ -10808,7 +10898,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>6</v>
@@ -10817,7 +10907,7 @@
         <v>2009</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>2009</v>
@@ -10825,7 +10915,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>6</v>
@@ -10834,7 +10924,7 @@
         <v>2019</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>2019</v>
@@ -10872,13 +10962,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1527480</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>129600</xdr:rowOff>
+                    <xdr:rowOff>114480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>429840</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>34200</xdr:rowOff>
+                    <xdr:rowOff>19080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10964,8 +11054,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10984,631 +11074,652 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>143</v>
       </c>
+      <c r="E1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>145</v>
+      </c>
       <c r="G1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>142</v>
+      <c r="I1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="13" t="b">
-        <v>1</v>
+      <c r="C2" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H2" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="14" t="n">
+      <c r="J2" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H3" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="14" t="n">
+      <c r="J3" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="13" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="H4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="14" t="n">
+      <c r="J4" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C5" s="13" t="b">
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="14" t="n">
+      <c r="E5" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="14" t="n">
+        <v>153</v>
+      </c>
+      <c r="H5" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="J5" s="14" t="n">
+      <c r="J5" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C6" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="14" t="n">
+      <c r="J6" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C7" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H7" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="14" t="n">
+      <c r="J7" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C8" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H8" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="14" t="n">
+      <c r="J8" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C9" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H9" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="14" t="n">
+      <c r="J9" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C10" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H10" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="14" t="n">
+      <c r="J10" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C11" s="13" t="b">
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="14" t="n">
+      <c r="E11" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H11" s="14" t="n">
+        <v>160</v>
+      </c>
+      <c r="H11" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="J11" s="14" t="n">
+      <c r="J11" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C12" s="13" t="b">
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="14" t="n">
+      <c r="E12" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H12" s="14" t="n">
+        <v>160</v>
+      </c>
+      <c r="H12" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="J12" s="14" t="n">
+      <c r="J12" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H13" s="14" t="n">
+      <c r="H13" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="J13" s="14" t="n">
+      <c r="J13" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C14" s="13" t="b">
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H14" s="14" t="n">
+        <v>160</v>
+      </c>
+      <c r="H14" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="J14" s="14" t="n">
+      <c r="J14" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C15" s="13" t="b">
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H15" s="14" t="n">
+        <v>160</v>
+      </c>
+      <c r="H15" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="J15" s="14" t="n">
+      <c r="J15" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C16" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">D11</f>
         <v>0</v>
       </c>
-      <c r="E16" s="14" t="n">
+      <c r="E16" s="12" t="n">
         <v>-0.23</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H16" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="14" t="n">
+      <c r="J16" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C17" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">D12</f>
         <v>0</v>
       </c>
-      <c r="E17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="10"/>
+      <c r="E17" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9"/>
       <c r="G17" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H17" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="14" t="n">
+      <c r="J17" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C18" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">D13</f>
         <v>0</v>
       </c>
-      <c r="E18" s="14" t="n">
+      <c r="E18" s="12" t="n">
         <v>-0.27</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H18" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="14" t="n">
+      <c r="J18" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C19" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">D14</f>
         <v>0</v>
       </c>
-      <c r="E19" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="10"/>
+      <c r="E19" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9"/>
       <c r="G19" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H19" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="14" t="n">
+      <c r="J19" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C20" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">D15</f>
         <v>0</v>
       </c>
-      <c r="E20" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="10"/>
+      <c r="E20" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H20" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="14" t="n">
+      <c r="J20" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C21" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="10" t="s">
+      <c r="E21" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H21" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J21" s="14" t="n">
+      <c r="J21" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C22" s="15" t="b">
+        <v>171</v>
+      </c>
+      <c r="C22" s="13" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="10" t="s">
+      <c r="E22" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H22" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="14" t="n">
+      <c r="J22" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C23" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.33</v>
       </c>
-      <c r="E23" s="14" t="n">
+      <c r="E23" s="12" t="n">
         <v>0.33</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H23" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="14" t="n">
+      <c r="J23" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="5" t="n">
+      <c r="A24" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="4" t="n">
         <v>0.7</v>
       </c>
-      <c r="E24" s="16" t="n">
+      <c r="E24" s="14" t="n">
         <v>0.7</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="H24" s="16" t="s">
+      <c r="G24" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="16" t="n">
+      <c r="I24" s="4"/>
+      <c r="J24" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11662,7 +11773,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>-309960</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>28440</xdr:rowOff>
+                    <xdr:rowOff>12960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12142,10 +12253,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12165,83 +12276,66 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>123</v>
+        <v>175</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.45</v>
+        <v>0.83115</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.83115</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.83115</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>177</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.83115</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>179</v>
+        <v>0.35</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>182</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" s="0" t="n">
         <v>0.35</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.35</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2" type="list">
-      <formula1>"Trend"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -12257,15 +12351,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66.57"/>
   </cols>
@@ -12284,80 +12378,104 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>183</v>
+      <c r="C2" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>186</v>
+      <c r="C3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="8" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>188</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>25</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B5" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="0" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C6" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="D6" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>2018</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3" type="list">
       <formula1>"Constant,Trend"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2" type="list">
       <formula1>"Historical,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
+      <formula1>"Reference,User"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -12380,15 +12498,15 @@
                 <anchor moveWithCells="true" sizeWithCells="false">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>453600</xdr:colOff>
+                    <xdr:colOff>654840</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>15120</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>-612360</xdr:colOff>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>-411120</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>-54720</xdr:rowOff>
+                    <xdr:rowOff>-69840</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12432,14 +12550,14 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="8" t="b">
+        <v>131</v>
+      </c>
+      <c r="C2" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12449,14 +12567,14 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="8" t="b">
+        <v>195</v>
+      </c>
+      <c r="C3" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>25</v>
@@ -12464,18 +12582,18 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
@@ -12484,7 +12602,7 @@
         <v>2019</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>2019</v>
@@ -12492,7 +12610,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>6</v>
@@ -12501,7 +12619,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.5</v>
@@ -12535,7 +12653,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>6840</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>34200</xdr:rowOff>
+                    <xdr:rowOff>19080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12590,89 +12708,89 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>194</v>
+      <c r="C1" s="10" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="15" t="b">
+      <c r="C2" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="15" t="b">
+      <c r="C3" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="15" t="b">
+      <c r="C4" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="15" t="b">
+      <c r="C5" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="15" t="b">
+      <c r="C6" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="15" t="b">
+      <c r="C7" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="15" t="b">
+      <c r="C8" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="15" t="b">
+      <c r="C9" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="15" t="b">
+      <c r="C10" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="15" t="b">
+      <c r="C11" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="15" t="b">
+      <c r="C12" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="15" t="b">
+      <c r="C13" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="15" t="b">
+      <c r="C14" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12705,7 +12823,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>-501480</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>28080</xdr:rowOff>
+                    <xdr:rowOff>12600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
lots of fixed, especially regardign specific consumption, started splitting nuts2 from historical data and started using docstrings
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -759,7 +759,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -816,10 +816,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1085,7 +1081,7 @@
   </sheetPr>
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1285,7 +1281,7 @@
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="8" t="b">
+      <c r="C21" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1294,7 +1290,7 @@
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="8" t="b">
+      <c r="C22" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1303,7 +1299,7 @@
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="8" t="b">
+      <c r="C23" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1312,7 +1308,7 @@
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="8" t="b">
+      <c r="C24" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1321,7 +1317,7 @@
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="8" t="b">
+      <c r="C25" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1330,7 +1326,7 @@
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="8" t="b">
+      <c r="C26" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1339,7 +1335,7 @@
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="8" t="b">
+      <c r="C27" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1348,7 +1344,7 @@
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="8" t="b">
+      <c r="C28" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1357,7 +1353,7 @@
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="8" t="b">
+      <c r="C29" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1366,7 +1362,7 @@
       <c r="A30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="8" t="b">
+      <c r="C30" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1375,7 +1371,7 @@
       <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="8" t="b">
+      <c r="C31" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1384,7 +1380,7 @@
       <c r="A32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="8" t="b">
+      <c r="C32" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1393,7 +1389,7 @@
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="8" t="b">
+      <c r="C33" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1402,7 +1398,7 @@
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="8" t="b">
+      <c r="C34" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1411,7 +1407,7 @@
       <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="8" t="b">
+      <c r="C35" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1420,7 +1416,7 @@
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="8" t="b">
+      <c r="C36" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1432,7 +1428,7 @@
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="8" t="b">
+      <c r="C37" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1444,7 +1440,7 @@
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="8" t="b">
+      <c r="C38" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1453,7 +1449,7 @@
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="8" t="b">
+      <c r="C39" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1462,7 +1458,7 @@
       <c r="A40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="8" t="b">
+      <c r="C40" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1471,7 +1467,7 @@
       <c r="A41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="8" t="b">
+      <c r="C41" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1480,7 +1476,7 @@
       <c r="A42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="8" t="b">
+      <c r="C42" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1489,7 +1485,7 @@
       <c r="A43" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="8" t="b">
+      <c r="C43" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1498,7 +1494,7 @@
       <c r="A44" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="8" t="b">
+      <c r="C44" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1507,7 +1503,7 @@
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="8" t="b">
+      <c r="C45" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1516,7 +1512,7 @@
       <c r="A46" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="8" t="b">
+      <c r="C46" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1525,7 +1521,7 @@
       <c r="A47" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="8" t="b">
+      <c r="C47" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1534,7 +1530,7 @@
       <c r="A48" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="8" t="b">
+      <c r="C48" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1543,7 +1539,7 @@
       <c r="A49" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="8" t="b">
+      <c r="C49" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1552,7 +1548,7 @@
       <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="8" t="b">
+      <c r="C50" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1561,7 +1557,7 @@
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="8" t="b">
+      <c r="C51" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1570,7 +1566,7 @@
       <c r="A52" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="8" t="b">
+      <c r="C52" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1579,7 +1575,7 @@
       <c r="A53" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="8" t="b">
+      <c r="C53" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1588,7 +1584,7 @@
       <c r="A54" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="8" t="b">
+      <c r="C54" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1597,7 +1593,7 @@
       <c r="A55" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="8" t="b">
+      <c r="C55" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1606,7 +1602,7 @@
       <c r="A56" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="8" t="b">
+      <c r="C56" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1615,7 +1611,7 @@
       <c r="A57" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="8" t="b">
+      <c r="C57" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1624,7 +1620,7 @@
       <c r="A58" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="8" t="b">
+      <c r="C58" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1633,7 +1629,7 @@
       <c r="A59" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="8" t="b">
+      <c r="C59" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1918,7 +1914,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1977,13 +1973,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="8" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>130</v>
@@ -2061,7 +2057,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>139</v>
@@ -2160,7 +2156,7 @@
       <c r="D2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="14" t="n">
+      <c r="E2" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="10" t="s">
@@ -2169,10 +2165,10 @@
       <c r="G2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="14" t="n">
+      <c r="H2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2188,7 +2184,7 @@
       <c r="D3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="14" t="n">
+      <c r="E3" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2197,10 +2193,10 @@
       <c r="G3" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="14" t="n">
+      <c r="H3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2215,7 +2211,7 @@
       <c r="D4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -2224,10 +2220,10 @@
       <c r="G4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="14" t="n">
+      <c r="H4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2242,7 +2238,7 @@
       <c r="D5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="14" t="n">
+      <c r="E5" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
@@ -2251,10 +2247,10 @@
       <c r="G5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H5" s="14" t="n">
+      <c r="H5" s="13" t="n">
         <v>60</v>
       </c>
-      <c r="J5" s="14" t="n">
+      <c r="J5" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2269,7 +2265,7 @@
       <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -2278,10 +2274,10 @@
       <c r="G6" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="14" t="n">
+      <c r="H6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2296,7 +2292,7 @@
       <c r="D7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -2305,10 +2301,10 @@
       <c r="G7" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="14" t="n">
+      <c r="H7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2323,7 +2319,7 @@
       <c r="D8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E8" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F8" s="10" t="s">
@@ -2332,10 +2328,10 @@
       <c r="G8" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="14" t="n">
+      <c r="H8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2350,7 +2346,7 @@
       <c r="D9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="14" t="n">
+      <c r="E9" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="10" t="s">
@@ -2359,10 +2355,10 @@
       <c r="G9" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="14" t="n">
+      <c r="H9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2377,7 +2373,7 @@
       <c r="D10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="14" t="n">
+      <c r="E10" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -2386,10 +2382,10 @@
       <c r="G10" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="14" t="n">
+      <c r="H10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2404,7 +2400,7 @@
       <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="14" t="n">
+      <c r="E11" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="1" t="n">
@@ -2413,10 +2409,10 @@
       <c r="G11" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H11" s="14" t="n">
+      <c r="H11" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="J11" s="14" t="n">
+      <c r="J11" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2431,7 +2427,7 @@
       <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="14" t="n">
+      <c r="E12" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="1" t="n">
@@ -2440,10 +2436,10 @@
       <c r="G12" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H12" s="14" t="n">
+      <c r="H12" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="J12" s="14" t="n">
+      <c r="J12" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2458,7 +2454,7 @@
       <c r="D13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="14" t="n">
+      <c r="E13" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="1" t="n">
@@ -2467,10 +2463,10 @@
       <c r="G13" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H13" s="14" t="n">
+      <c r="H13" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="J13" s="14" t="n">
+      <c r="J13" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2485,7 +2481,7 @@
       <c r="D14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="1" t="n">
@@ -2494,10 +2490,10 @@
       <c r="G14" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H14" s="14" t="n">
+      <c r="H14" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="J14" s="14" t="n">
+      <c r="J14" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2512,7 +2508,7 @@
       <c r="D15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="1" t="n">
@@ -2521,10 +2517,10 @@
       <c r="G15" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H15" s="14" t="n">
+      <c r="H15" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="J15" s="14" t="n">
+      <c r="J15" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2540,17 +2536,17 @@
         <f aca="false">D11</f>
         <v>0</v>
       </c>
-      <c r="E16" s="14" t="n">
+      <c r="E16" s="13" t="n">
         <v>-0.23</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="14" t="n">
+      <c r="H16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2566,17 +2562,17 @@
         <f aca="false">D12</f>
         <v>0</v>
       </c>
-      <c r="E17" s="14" t="n">
+      <c r="E17" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="14" t="n">
+      <c r="H17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2592,17 +2588,17 @@
         <f aca="false">D13</f>
         <v>0</v>
       </c>
-      <c r="E18" s="14" t="n">
+      <c r="E18" s="13" t="n">
         <v>-0.27</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="14" t="n">
+      <c r="H18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2618,17 +2614,17 @@
         <f aca="false">D14</f>
         <v>0</v>
       </c>
-      <c r="E19" s="14" t="n">
+      <c r="E19" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="14" t="n">
+      <c r="H19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2644,17 +2640,17 @@
         <f aca="false">D15</f>
         <v>0</v>
       </c>
-      <c r="E20" s="14" t="n">
+      <c r="E20" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H20" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="14" t="n">
+      <c r="H20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2669,7 +2665,7 @@
       <c r="D21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="14" t="n">
+      <c r="E21" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="10" t="s">
@@ -2678,10 +2674,10 @@
       <c r="G21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H21" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="14" t="n">
+      <c r="H21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2696,7 +2692,7 @@
       <c r="D22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="14" t="n">
+      <c r="E22" s="13" t="n">
         <v>0</v>
       </c>
       <c r="F22" s="10" t="s">
@@ -2705,10 +2701,10 @@
       <c r="G22" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J22" s="14" t="n">
+      <c r="H22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2723,7 +2719,7 @@
       <c r="D23" s="1" t="n">
         <v>0.33</v>
       </c>
-      <c r="E23" s="14" t="n">
+      <c r="E23" s="13" t="n">
         <v>0.33</v>
       </c>
       <c r="F23" s="10" t="s">
@@ -2732,10 +2728,10 @@
       <c r="G23" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H23" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="14" t="n">
+      <c r="H23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2746,11 +2742,11 @@
       <c r="B24" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="E24" s="15" t="n">
+      <c r="E24" s="14" t="n">
         <v>0.7</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -2759,11 +2755,11 @@
       <c r="G24" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="14" t="s">
         <v>6</v>
       </c>
       <c r="I24" s="5"/>
-      <c r="J24" s="15" t="n">
+      <c r="J24" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3189,79 +3185,79 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="14" t="b">
+      <c r="C2" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="14" t="b">
+      <c r="C3" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="14" t="b">
+      <c r="C4" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="14" t="b">
+      <c r="C5" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="14" t="b">
+      <c r="C6" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="14" t="b">
+      <c r="C7" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="14" t="b">
+      <c r="C8" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="14" t="b">
+      <c r="C9" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="14" t="b">
+      <c r="C10" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="14" t="b">
+      <c r="C11" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="14" t="b">
+      <c r="C12" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="14" t="b">
+      <c r="C13" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="14" t="b">
+      <c r="C14" s="13" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
advancement on reading nuts2 data
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -1281,7 +1281,7 @@
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="1" t="b">
+      <c r="C21" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1290,7 +1290,7 @@
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="1" t="b">
+      <c r="C22" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="1" t="b">
+      <c r="C23" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="1" t="b">
+      <c r="C24" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="1" t="b">
+      <c r="C25" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="1" t="b">
+      <c r="C26" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="1" t="b">
+      <c r="C27" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="1" t="b">
+      <c r="C28" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1353,7 +1353,7 @@
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="1" t="b">
+      <c r="C29" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1362,7 +1362,7 @@
       <c r="A30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="1" t="b">
+      <c r="C30" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1371,7 +1371,7 @@
       <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="1" t="b">
+      <c r="C31" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1380,7 +1380,7 @@
       <c r="A32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="1" t="b">
+      <c r="C32" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="1" t="b">
+      <c r="C33" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="1" t="b">
+      <c r="C34" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="1" t="b">
+      <c r="C35" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="1" t="b">
+      <c r="C36" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="1" t="b">
+      <c r="C37" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1440,7 +1440,7 @@
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="1" t="b">
+      <c r="C38" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="1" t="b">
+      <c r="C39" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="A40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="1" t="b">
+      <c r="C40" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1467,7 +1467,7 @@
       <c r="A41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="1" t="b">
+      <c r="C41" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1476,7 +1476,7 @@
       <c r="A42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="1" t="b">
+      <c r="C42" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="A43" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="1" t="b">
+      <c r="C43" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1494,7 +1494,7 @@
       <c r="A44" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="1" t="b">
+      <c r="C44" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1503,7 +1503,7 @@
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="1" t="b">
+      <c r="C45" s="8" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1914,7 +1914,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2057,7 +2057,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
cts sector now really done (same values as reference)
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\Master_Semester_1\IDP\endemo2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F26066F-5535-44C6-A6D7-71BE69485E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266D79C4-D3CA-4350-9EB7-274FD6579C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4010" yWindow="2100" windowWidth="19200" windowHeight="11260" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="2100" windowWidth="19200" windowHeight="11260" tabRatio="730" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
   <si>
     <t>Country</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Activates calculations for commertial, trade and services sector.</t>
   </si>
   <si>
-    <t>Has to be active at least for the first forecast calculation.</t>
-  </si>
-  <si>
     <t>Forecast of load profiles. If false, just yearly values are calculated.</t>
   </si>
   <si>
@@ -389,12 +386,6 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>World calculation</t>
-  </si>
-  <si>
-    <t>If a country outside of Europe is calculated.</t>
-  </si>
-  <si>
     <t>Brunei Darussalam</t>
   </si>
   <si>
@@ -693,6 +684,9 @@
   </si>
   <si>
     <t>Linear time trend</t>
+  </si>
+  <si>
+    <t>If NUTS2 resolution is activated, population forecast has to be active at least for the first calculation.</t>
   </si>
 </sst>
 </file>
@@ -801,9 +795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -816,6 +807,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,119 +832,119 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp100.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp108.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp109.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp111.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp112.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp108.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp109.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C2" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp111.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp112.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp126.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,171 +952,167 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp127.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp128.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp129.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp130.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp131.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp132.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp133.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp134.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp135.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp136.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp137.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp138.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp139.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1130,43 +1120,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$39" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$39" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$41" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1174,219 +1164,219 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp50.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$41" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$43" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$43" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$44" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$44" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$45" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp54.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$45" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$46" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$46" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$47" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$47" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$54" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$54" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$52" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$52" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$51" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp59.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$51" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$55" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$55" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$56" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$56" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$57" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$57" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$58" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$58" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$59" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$59" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$60" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$60" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$50" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$50" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$49" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$49" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$61" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$61" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$66" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$66" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$67" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$67" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$68" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$68" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$69" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$69" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$70" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$70" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$71" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$71" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$72" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$72" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$73" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$74" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$75" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$76" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$77" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$78" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$79" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$80" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$81" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$82" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$83" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$73" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$74" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$75" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$76" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$77" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$78" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$79" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$80" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$81" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$82" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp90.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$83" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$84" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp91.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$84" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$85" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp92.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$85" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$86" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp93.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$86" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$87" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp94.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$87" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$88" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$88" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$53" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp96.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$53" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$48" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$48" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1999,13 +1989,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2085,99 +2075,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2060" name="Check Box 12" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2060"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>13</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -13655,10 +13559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13699,10 +13603,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="5">
-        <v>2018</v>
+        <v>2050</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="5">
         <v>2050</v>
@@ -13727,7 +13631,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
@@ -13741,7 +13645,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -13772,7 +13676,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>56</v>
@@ -13783,10 +13687,10 @@
         <v>50</v>
       </c>
       <c r="C8" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>56</v>
@@ -13797,77 +13701,64 @@
         <v>51</v>
       </c>
       <c r="C9" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>73</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2016</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2016</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2016</v>
-      </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="5">
-        <v>2016</v>
+      <c r="A11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{84BA2A67-2FC3-451D-BC2B-A22C158F230C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{84BA2A67-2FC3-451D-BC2B-A22C158F230C}">
       <formula1>"2016, 2021"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14040,13 +13931,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>12700</xdr:colOff>
-                    <xdr:row>11</xdr:row>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1143000</xdr:colOff>
-                    <xdr:row>12</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -14056,41 +13947,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2060" r:id="rId12" name="Check Box 12">
+            <control shapeId="2061" r:id="rId12" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>12700</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1143000</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2061" r:id="rId13" name="Check Box 13">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>1143000</xdr:colOff>
-                    <xdr:row>13</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -14108,7 +13977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -14146,7 +14015,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -14162,7 +14031,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -14170,7 +14039,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -14178,7 +14047,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -14186,7 +14055,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -14194,7 +14063,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -14202,7 +14071,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -14210,7 +14079,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -14218,7 +14087,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -14226,7 +14095,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -14234,7 +14103,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -14242,7 +14111,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -14250,7 +14119,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -14258,7 +14127,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -14266,7 +14135,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -14274,7 +14143,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -14282,7 +14151,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -14290,7 +14159,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -14298,7 +14167,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -14306,7 +14175,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -14314,7 +14183,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -14322,7 +14191,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -14330,7 +14199,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -14338,7 +14207,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -14346,7 +14215,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -14354,7 +14223,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -14362,7 +14231,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -14370,7 +14239,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -14378,7 +14247,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -14386,7 +14255,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -14394,7 +14263,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -14402,7 +14271,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -14424,12 +14293,12 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -14437,7 +14306,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -14445,7 +14314,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -14453,7 +14322,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -14461,7 +14330,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -14469,7 +14338,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -14477,7 +14346,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -14485,7 +14354,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -14493,7 +14362,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -14501,7 +14370,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -14509,7 +14378,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -14517,7 +14386,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -14525,7 +14394,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -14533,7 +14402,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -14541,7 +14410,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -14549,7 +14418,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -14557,7 +14426,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -14565,7 +14434,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -14573,7 +14442,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -14581,7 +14450,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -14589,7 +14458,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -14597,7 +14466,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -14605,7 +14474,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -14613,7 +14482,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -14621,7 +14490,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -14629,7 +14498,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -14637,7 +14506,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -14645,7 +14514,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -14653,7 +14522,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -14661,7 +14530,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -14669,7 +14538,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -14677,7 +14546,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -14685,7 +14554,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -14693,7 +14562,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -14701,7 +14570,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -14709,7 +14578,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
@@ -14717,7 +14586,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
@@ -14725,7 +14594,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -14733,7 +14602,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -14741,7 +14610,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -14749,7 +14618,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -14757,7 +14626,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
@@ -14765,7 +14634,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
@@ -14773,7 +14642,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -14781,7 +14650,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
@@ -14789,7 +14658,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
@@ -14797,7 +14666,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
@@ -14805,7 +14674,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
@@ -14813,7 +14682,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -14821,7 +14690,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
@@ -14829,7 +14698,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C88" t="b">
         <v>0</v>
@@ -16797,44 +16666,44 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
         <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -16842,7 +16711,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -16853,13 +16722,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>56</v>
@@ -16867,7 +16736,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
@@ -16876,7 +16745,7 @@
         <v>2009</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7">
         <v>2009</v>
@@ -16884,50 +16753,50 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>2019</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8">
         <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E9" s="13">
+      <c r="D9" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -16935,16 +16804,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B11" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -16952,16 +16821,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B12" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -16969,16 +16838,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>205</v>
-      </c>
-      <c r="B13" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -16986,16 +16855,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -17003,16 +16872,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -17020,16 +16889,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B16" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -17147,7 +17016,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17166,39 +17035,39 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>180</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="b">
@@ -17210,11 +17079,11 @@
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>44</v>
@@ -17228,11 +17097,11 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -17240,11 +17109,11 @@
       <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>44</v>
@@ -17258,10 +17127,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -17269,11 +17138,11 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>44</v>
@@ -17287,10 +17156,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -17299,10 +17168,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H5" s="4">
         <v>100</v>
@@ -17316,7 +17185,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>1</v>
@@ -17327,11 +17196,11 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>44</v>
@@ -17345,7 +17214,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
@@ -17356,11 +17225,11 @@
       <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>44</v>
@@ -17374,7 +17243,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
@@ -17385,11 +17254,11 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>44</v>
@@ -17403,7 +17272,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>1</v>
@@ -17414,11 +17283,11 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>44</v>
@@ -17432,7 +17301,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>1</v>
@@ -17443,11 +17312,11 @@
       <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>44</v>
@@ -17461,7 +17330,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="4" t="b">
         <v>1</v>
@@ -17477,7 +17346,7 @@
         <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H11" s="4">
         <v>100</v>
@@ -17491,7 +17360,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4" t="b">
         <v>1</v>
@@ -17507,7 +17376,7 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H12" s="4">
         <v>100</v>
@@ -17521,7 +17390,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="4" t="b">
         <v>1</v>
@@ -17537,7 +17406,7 @@
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H13" s="4">
         <v>100</v>
@@ -17551,7 +17420,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="4" t="b">
         <v>1</v>
@@ -17567,7 +17436,7 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H14" s="4">
         <v>100</v>
@@ -17581,7 +17450,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="4" t="b">
         <v>1</v>
@@ -17597,7 +17466,7 @@
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H15" s="4">
         <v>100</v>
@@ -17611,7 +17480,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C16" s="4" t="b">
         <v>1</v>
@@ -17623,12 +17492,12 @@
       <c r="E16" s="4">
         <v>-0.23</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <f>100-F11</f>
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H16" s="4">
         <v>0</v>
@@ -17642,7 +17511,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C17" s="4" t="b">
         <v>1</v>
@@ -17654,12 +17523,12 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <f t="shared" ref="F17:F20" si="2">100-F12</f>
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H17" s="4">
         <v>0</v>
@@ -17673,7 +17542,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C18" s="4" t="b">
         <v>1</v>
@@ -17685,12 +17554,12 @@
       <c r="E18" s="4">
         <v>-0.27</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H18" s="4">
         <v>0</v>
@@ -17704,7 +17573,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C19" s="4" t="b">
         <v>1</v>
@@ -17716,12 +17585,12 @@
       <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
@@ -17735,7 +17604,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C20" s="4" t="b">
         <v>1</v>
@@ -17747,12 +17616,12 @@
       <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
@@ -17766,7 +17635,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="4" t="b">
         <v>1</v>
@@ -17777,11 +17646,11 @@
       <c r="E21" s="4">
         <v>0</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>44</v>
@@ -17795,7 +17664,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="4" t="b">
         <v>1</v>
@@ -17806,11 +17675,11 @@
       <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>44</v>
@@ -17824,7 +17693,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="4" t="b">
         <v>1</v>
@@ -17835,11 +17704,11 @@
       <c r="E23" s="4">
         <v>0.33</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>44</v>
@@ -17853,31 +17722,31 @@
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="9"/>
+        <v>181</v>
+      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="6">
         <v>0.7</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>0.7</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="H24" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>44</v>
       </c>
       <c r="I24" s="6">
         <v>0</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>0</v>
       </c>
     </row>
@@ -18419,41 +18288,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>0.45</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2">
         <v>0.45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="11">
         <v>0.83115000000000006</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="12">
+      <c r="C3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="11">
         <v>0.83115000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -18461,13 +18330,13 @@
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -18475,13 +18344,13 @@
     </row>
     <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -18527,72 +18396,72 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -18601,7 +18470,7 @@
         <v>2018</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6">
         <v>2018</v>
@@ -18657,8 +18526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18686,10 +18555,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>56</v>
@@ -18697,32 +18566,32 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>104</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -18731,7 +18600,7 @@
         <v>2019</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5">
         <v>2019</v>
@@ -18739,7 +18608,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -18748,41 +18617,41 @@
         <v>0.5</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="13">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -18863,13 +18732,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
large part of households sector
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\Master_Semester_1\IDP\endemo2\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tumde-my.sharepoint.com/personal/chris_kobalt_tum_de/Documents/Documents/Master_Semester_1/IDP/endemo2/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266D79C4-D3CA-4350-9EB7-274FD6579C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F4AF2F6B-3CB2-4AC1-B816-49962119F171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A7D06FD-0E50-4190-BEF6-8BEE3D5257D6}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="2100" windowWidth="19200" windowHeight="11260" tabRatio="730" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14740" windowHeight="11260" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -828,7 +828,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1072,7 +1072,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1116,7 +1116,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13561,8 +13561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13617,7 +13617,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
@@ -13645,7 +13645,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -13659,7 +13659,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -18263,7 +18263,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18526,8 +18526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
documentation and uses now datapoints instead of float tuples
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\OneDrive - TUM\Documents\Master_Semester_1\IDP\endemo2\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\endemo\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B65F35-0F51-486D-A497-B2B6D1D941B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC9625F-0598-4EB5-890D-C3A1370DCC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="1740" windowWidth="16815" windowHeight="11595" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,9 @@
   <commentList>
     <comment ref="A2" authorId="0" shapeId="0" xr:uid="{04D4C06B-8268-4FCD-9269-B3F03D9D6D63}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     Refers to the sum of primary and secondary steel. If "steel" is activated, steel_prim and steel_sec should not be additionally activated and the other way round.</t>
       </text>
     </comment>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="211">
   <si>
     <t>Country</t>
   </si>
@@ -248,6 +248,9 @@
     <t>Activates calculations for commertial, trade and services sector.</t>
   </si>
   <si>
+    <t>Has to be active at least for the first forecast calculation.</t>
+  </si>
+  <si>
     <t>Forecast of load profiles. If false, just yearly values are calculated.</t>
   </si>
   <si>
@@ -386,6 +389,12 @@
     <t>Indonesia</t>
   </si>
   <si>
+    <t>World calculation</t>
+  </si>
+  <si>
+    <t>If a country outside of Europe is calculated.</t>
+  </si>
+  <si>
     <t>Brunei Darussalam</t>
   </si>
   <si>
@@ -684,9 +693,6 @@
   </si>
   <si>
     <t>Linear time trend</t>
-  </si>
-  <si>
-    <t>If NUTS2 resolution is activated, population forecast has to be active at least for the first calculation.</t>
   </si>
 </sst>
 </file>
@@ -795,6 +801,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -807,12 +816,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -828,123 +834,123 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp100.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp108.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp109.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C2" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp100.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp111.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp112.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp108.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp109.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp111.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp112.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp126.xml><?xml version="1.0" encoding="utf-8"?>
@@ -952,123 +958,127 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp127.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp128.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp128.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp129.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp129.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp130.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp130.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp131.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp131.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp132.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp132.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp133.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp133.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp134.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp134.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp135.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp135.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp136.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp136.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp137.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp137.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp138.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp138.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp139.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1076,43 +1086,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1120,43 +1130,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$37" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$38" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$39" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$40" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$41" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1164,219 +1174,219 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp50.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$41" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$42" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$43" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$44" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp54.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$45" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$46" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$47" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$54" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$52" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp59.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$51" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$55" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$56" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$57" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$58" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$59" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$60" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$50" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$49" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$62" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$61" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$63" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$64" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$65" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$66" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$67" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$68" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$69" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$70" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$71" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$72" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$73" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$74" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$75" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$76" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$77" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$78" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$79" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$80" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$81" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$82" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp90.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$83" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp90.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp91.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$84" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp92.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$85" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp93.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$86" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp94.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$87" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$88" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp96.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$53" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$48" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1450,7 +1460,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1536,7 +1546,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1622,7 +1632,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1708,7 +1718,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1794,7 +1804,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1880,7 +1890,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1966,7 +1976,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1989,13 +1999,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>12</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2052,7 +2062,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2075,24 +2085,24 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2061" name="Check Box 13" hidden="1">
+            <xdr:cNvPr id="2060" name="Check Box 12" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2061"/>
+                  <a14:compatExt spid="_x0000_s2060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D080000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2138,7 +2148,93 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Activate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1143000</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2061" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2061"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2229,7 +2325,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2315,7 +2411,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2401,7 +2497,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2487,7 +2583,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2573,7 +2669,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2659,7 +2755,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2745,7 +2841,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2831,7 +2927,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2917,7 +3013,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3003,7 +3099,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3089,7 +3185,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3175,7 +3271,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3261,7 +3357,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3347,7 +3443,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3433,7 +3529,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3519,7 +3615,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3605,7 +3701,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3691,7 +3787,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3777,7 +3873,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3863,7 +3959,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3949,7 +4045,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4035,7 +4131,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4121,7 +4217,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4207,7 +4303,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4293,7 +4389,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4379,7 +4475,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4465,7 +4561,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4551,7 +4647,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4637,7 +4733,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4723,7 +4819,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4809,7 +4905,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4895,7 +4991,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4981,7 +5077,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5067,7 +5163,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5153,7 +5249,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5239,7 +5335,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5325,7 +5421,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5411,7 +5507,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5497,7 +5593,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5583,7 +5679,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5669,7 +5765,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5755,7 +5851,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5841,7 +5937,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5927,7 +6023,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6013,7 +6109,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6099,7 +6195,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6185,7 +6281,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6271,7 +6367,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6357,7 +6453,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6443,7 +6539,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6529,7 +6625,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6615,7 +6711,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6701,7 +6797,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6787,7 +6883,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6873,7 +6969,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6959,7 +7055,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7045,7 +7141,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7131,7 +7227,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7217,7 +7313,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7303,7 +7399,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7389,7 +7485,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7475,7 +7571,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7561,7 +7657,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7647,7 +7743,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7733,7 +7829,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7819,7 +7915,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7905,7 +8001,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7991,7 +8087,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8077,7 +8173,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8163,7 +8259,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8249,7 +8345,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8335,7 +8431,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8421,7 +8517,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8507,7 +8603,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8593,7 +8689,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8679,7 +8775,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8765,7 +8861,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8851,7 +8947,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8937,7 +9033,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9023,7 +9119,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9109,7 +9205,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9195,7 +9291,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9281,7 +9377,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9367,7 +9463,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9453,7 +9549,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9539,7 +9635,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9625,7 +9721,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9716,7 +9812,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9802,7 +9898,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9888,7 +9984,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -9974,7 +10070,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10065,7 +10161,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10151,7 +10247,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10237,7 +10333,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10323,7 +10419,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10409,7 +10505,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10495,7 +10591,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10581,7 +10677,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10667,7 +10763,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10753,7 +10849,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10839,7 +10935,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -10925,7 +11021,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11011,7 +11107,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11097,7 +11193,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11183,7 +11279,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11269,7 +11365,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11355,7 +11451,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11441,7 +11537,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11527,7 +11623,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11613,7 +11709,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11699,7 +11795,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11785,7 +11881,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11871,7 +11967,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -11962,7 +12058,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12053,7 +12149,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12139,7 +12235,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12230,7 +12326,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12316,7 +12412,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12402,7 +12498,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12488,7 +12584,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12574,7 +12670,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12660,7 +12756,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12746,7 +12842,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12832,7 +12928,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -12918,7 +13014,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -13004,7 +13100,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -13090,7 +13186,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -13176,7 +13272,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -13262,7 +13358,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-AT" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -13559,13 +13655,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -13603,10 +13699,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="5">
-        <v>2050</v>
+        <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E2" s="5">
         <v>2050</v>
@@ -13617,7 +13713,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
@@ -13631,7 +13727,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
@@ -13676,7 +13772,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>208</v>
+        <v>62</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>56</v>
@@ -13687,10 +13783,10 @@
         <v>50</v>
       </c>
       <c r="C8" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>56</v>
@@ -13701,64 +13797,77 @@
         <v>51</v>
       </c>
       <c r="C9" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="5">
-        <v>2016</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="5">
-        <v>2016</v>
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>56</v>
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2016</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2016</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>187</v>
+        <v>53</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>76</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{84BA2A67-2FC3-451D-BC2B-A22C158F230C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{84BA2A67-2FC3-451D-BC2B-A22C158F230C}">
       <formula1>"2016, 2021"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13931,13 +14040,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>10</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1143000</xdr:colOff>
-                    <xdr:row>11</xdr:row>
+                    <xdr:row>12</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -13947,19 +14056,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2061" r:id="rId12" name="Check Box 13">
+            <control shapeId="2060" r:id="rId12" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>11</xdr:row>
+                    <xdr:row>9</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1143000</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2061" r:id="rId13" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1143000</xdr:colOff>
+                    <xdr:row>13</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -13977,11 +14108,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
@@ -14055,7 +14186,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -14063,7 +14194,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -14071,7 +14202,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -14079,7 +14210,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -14087,7 +14218,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -14095,7 +14226,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -14103,7 +14234,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -14111,7 +14242,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -14119,7 +14250,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -14127,7 +14258,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -14135,7 +14266,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -14143,7 +14274,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -14151,7 +14282,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -14159,7 +14290,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -14167,7 +14298,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -14175,7 +14306,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -14183,7 +14314,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -14191,7 +14322,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -14199,7 +14330,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -14207,7 +14338,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -14215,7 +14346,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -14223,7 +14354,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -14231,7 +14362,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -14239,7 +14370,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -14247,7 +14378,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -14255,7 +14386,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -14263,7 +14394,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -14271,7 +14402,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -14293,12 +14424,12 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -14306,7 +14437,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -14314,7 +14445,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -14322,7 +14453,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -14330,7 +14461,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -14338,7 +14469,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -14346,7 +14477,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -14354,7 +14485,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -14362,7 +14493,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -14370,7 +14501,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -14378,7 +14509,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -14386,7 +14517,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -14394,7 +14525,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -14402,7 +14533,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -14410,7 +14541,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -14418,7 +14549,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -14426,7 +14557,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -14434,7 +14565,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -14442,7 +14573,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -14450,7 +14581,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -14458,7 +14589,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -14466,7 +14597,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -14474,7 +14605,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -14482,7 +14613,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -14490,7 +14621,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -14498,7 +14629,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -14506,7 +14637,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -14514,7 +14645,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -14522,7 +14653,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -14530,7 +14661,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -14538,7 +14669,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -14546,7 +14677,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -14554,7 +14685,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -14562,7 +14693,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -14570,7 +14701,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -14578,7 +14709,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
@@ -14586,7 +14717,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
@@ -14594,7 +14725,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -14602,7 +14733,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -14610,7 +14741,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -14618,7 +14749,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -14626,7 +14757,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
@@ -14634,7 +14765,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
@@ -14642,7 +14773,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -14650,7 +14781,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
@@ -14658,7 +14789,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
@@ -14666,7 +14797,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
@@ -14674,7 +14805,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
@@ -14682,7 +14813,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -14690,7 +14821,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
@@ -14698,7 +14829,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C88" t="b">
         <v>0</v>
@@ -16640,7 +16771,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
@@ -16666,44 +16797,44 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -16711,7 +16842,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -16722,13 +16853,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
         <v>56</v>
@@ -16736,7 +16867,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
@@ -16745,7 +16876,7 @@
         <v>2009</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E7">
         <v>2009</v>
@@ -16753,50 +16884,50 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="12">
         <v>2019</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E8">
         <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="D9" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B10" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -16804,16 +16935,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -16821,16 +16952,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B12" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -16838,16 +16969,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B13" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -16855,16 +16986,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>203</v>
-      </c>
-      <c r="B14" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -16872,16 +17003,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>204</v>
-      </c>
-      <c r="B15" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -16889,16 +17020,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B16" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -17016,10 +17147,10 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -17035,39 +17166,39 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>169</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>173</v>
+        <v>93</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>177</v>
+        <v>93</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="b">
@@ -17079,11 +17210,11 @@
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>44</v>
@@ -17097,11 +17228,11 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -17109,11 +17240,11 @@
       <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>44</v>
@@ -17127,10 +17258,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C4" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -17138,11 +17269,11 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>44</v>
@@ -17156,10 +17287,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -17168,10 +17299,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H5" s="4">
         <v>100</v>
@@ -17185,7 +17316,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>1</v>
@@ -17196,11 +17327,11 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>44</v>
@@ -17214,7 +17345,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
@@ -17225,11 +17356,11 @@
       <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>44</v>
@@ -17243,7 +17374,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
@@ -17254,11 +17385,11 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>44</v>
@@ -17272,7 +17403,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>1</v>
@@ -17283,11 +17414,11 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>44</v>
@@ -17301,7 +17432,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>1</v>
@@ -17312,11 +17443,11 @@
       <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>44</v>
@@ -17330,7 +17461,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11" s="4" t="b">
         <v>1</v>
@@ -17346,7 +17477,7 @@
         <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H11" s="4">
         <v>100</v>
@@ -17360,7 +17491,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C12" s="4" t="b">
         <v>1</v>
@@ -17376,7 +17507,7 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H12" s="4">
         <v>100</v>
@@ -17390,7 +17521,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C13" s="4" t="b">
         <v>1</v>
@@ -17406,7 +17537,7 @@
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H13" s="4">
         <v>100</v>
@@ -17420,7 +17551,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C14" s="4" t="b">
         <v>1</v>
@@ -17436,7 +17567,7 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H14" s="4">
         <v>100</v>
@@ -17450,7 +17581,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="4" t="b">
         <v>1</v>
@@ -17466,7 +17597,7 @@
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H15" s="4">
         <v>100</v>
@@ -17480,7 +17611,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C16" s="4" t="b">
         <v>1</v>
@@ -17492,12 +17623,12 @@
       <c r="E16" s="4">
         <v>-0.23</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="10">
         <f>100-F11</f>
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H16" s="4">
         <v>0</v>
@@ -17511,7 +17642,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C17" s="4" t="b">
         <v>1</v>
@@ -17523,12 +17654,12 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="10">
         <f t="shared" ref="F17:F20" si="2">100-F12</f>
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H17" s="4">
         <v>0</v>
@@ -17542,7 +17673,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C18" s="4" t="b">
         <v>1</v>
@@ -17554,12 +17685,12 @@
       <c r="E18" s="4">
         <v>-0.27</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H18" s="4">
         <v>0</v>
@@ -17573,7 +17704,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C19" s="4" t="b">
         <v>1</v>
@@ -17585,12 +17716,12 @@
       <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
@@ -17604,7 +17735,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C20" s="4" t="b">
         <v>1</v>
@@ -17616,12 +17747,12 @@
       <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
@@ -17635,7 +17766,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C21" s="4" t="b">
         <v>1</v>
@@ -17646,11 +17777,11 @@
       <c r="E21" s="4">
         <v>0</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>44</v>
@@ -17664,7 +17795,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" s="4" t="b">
         <v>1</v>
@@ -17675,11 +17806,11 @@
       <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>44</v>
@@ -17693,7 +17824,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C23" s="4" t="b">
         <v>1</v>
@@ -17704,11 +17835,11 @@
       <c r="E23" s="4">
         <v>0.33</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>44</v>
@@ -17722,31 +17853,31 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C24" s="8"/>
+        <v>184</v>
+      </c>
+      <c r="C24" s="9"/>
       <c r="D24" s="6">
         <v>0.7</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="9">
         <v>0.7</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="11" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="H24" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>44</v>
       </c>
       <c r="I24" s="6">
         <v>0</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="9">
         <v>0</v>
       </c>
     </row>
@@ -18263,10 +18394,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
@@ -18288,41 +18419,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2">
         <v>0.45</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2">
         <v>0.45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="11">
+      <c r="A3" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="12">
         <v>0.83115000000000006</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="C3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="12">
         <v>0.83115000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -18330,13 +18461,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -18344,13 +18475,13 @@
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -18370,7 +18501,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
@@ -18396,72 +18527,72 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
         <v>102</v>
-      </c>
-      <c r="E2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -18470,7 +18601,7 @@
         <v>2018</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E6">
         <v>2018</v>
@@ -18527,10 +18658,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.7109375" customWidth="1"/>
@@ -18555,10 +18686,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>56</v>
@@ -18566,32 +18697,32 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -18600,7 +18731,7 @@
         <v>2019</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5">
         <v>2019</v>
@@ -18608,7 +18739,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -18617,41 +18748,41 @@
         <v>0.5</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E6">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="12">
-        <v>0</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B8" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -18723,7 +18854,7 @@
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -18732,13 +18863,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
households finished and start of transport
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\endemo\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC9625F-0598-4EB5-890D-C3A1370DCC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD4CD7F-D53E-4EEC-86ED-A380657A7AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13335" yWindow="915" windowWidth="21495" windowHeight="14655" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
   <si>
     <t>Country</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Activates calculations for commertial, trade and services sector.</t>
   </si>
   <si>
-    <t>Has to be active at least for the first forecast calculation.</t>
-  </si>
-  <si>
     <t>Forecast of load profiles. If false, just yearly values are calculated.</t>
   </si>
   <si>
@@ -389,12 +386,6 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>World calculation</t>
-  </si>
-  <si>
-    <t>If a country outside of Europe is calculated.</t>
-  </si>
-  <si>
     <t>Brunei Darussalam</t>
   </si>
   <si>
@@ -693,6 +684,9 @@
   </si>
   <si>
     <t>Linear time trend</t>
+  </si>
+  <si>
+    <t>If NUTS2 resolution is activated, population forecast has to be active at least for the first calculation.</t>
   </si>
 </sst>
 </file>
@@ -801,9 +795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -816,6 +807,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -838,119 +832,119 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp100.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp108.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp109.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp111.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp112.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp108.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp109.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C2" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp111.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp112.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp126.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,215 +952,211 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp127.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp128.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp129.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp130.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp131.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp132.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp133.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp134.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp135.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp136.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp137.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp138.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp139.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$39" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$39" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$41" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1174,87 +1164,87 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp50.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$41" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$43" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$43" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$44" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$44" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$45" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp54.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$45" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$46" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$46" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$47" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$47" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$54" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$54" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$52" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$52" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$51" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp59.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$51" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$55" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$55" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$56" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$56" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$57" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$57" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$58" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$58" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$59" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$59" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$60" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$60" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$50" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$50" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$49" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$49" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$61" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$61" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1262,131 +1252,131 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$66" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$66" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$67" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$67" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$68" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$68" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$69" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$69" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$70" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$70" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$71" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$71" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$72" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$72" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$73" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$74" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$75" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$76" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$77" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$78" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$79" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$80" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$81" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$82" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$83" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$73" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$74" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$75" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$76" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$77" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$78" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$79" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$80" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$81" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$82" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp90.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$83" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$84" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp91.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$84" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$85" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp92.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$85" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$86" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp93.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$86" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$87" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp94.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$87" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$88" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$88" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$53" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp96.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$53" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$48" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$48" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1999,13 +1989,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2085,99 +2075,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2060" name="Check Box 12" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2060"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>13</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -13655,7 +13559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -13699,10 +13603,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="5">
-        <v>2018</v>
+        <v>2050</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="5">
         <v>2050</v>
@@ -13727,7 +13631,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
@@ -13741,7 +13645,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -13755,7 +13659,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -13772,7 +13676,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>56</v>
@@ -13783,10 +13687,10 @@
         <v>50</v>
       </c>
       <c r="C8" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>56</v>
@@ -13800,74 +13704,61 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>73</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2016</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2016</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2016</v>
-      </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="5">
-        <v>2016</v>
+      <c r="A11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{84BA2A67-2FC3-451D-BC2B-A22C158F230C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{84BA2A67-2FC3-451D-BC2B-A22C158F230C}">
       <formula1>"2016, 2021"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14040,13 +13931,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>11</xdr:row>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1143000</xdr:colOff>
-                    <xdr:row>12</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -14056,41 +13947,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2060" r:id="rId12" name="Check Box 12">
+            <control shapeId="2061" r:id="rId12" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1143000</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2061" r:id="rId13" name="Check Box 13">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>1143000</xdr:colOff>
-                    <xdr:row>13</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -14108,7 +13977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -14186,7 +14055,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -14194,7 +14063,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -14202,7 +14071,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -14210,7 +14079,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -14218,7 +14087,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -14226,7 +14095,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -14234,7 +14103,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -14242,7 +14111,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -14250,7 +14119,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -14258,7 +14127,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -14266,7 +14135,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -14274,7 +14143,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -14282,7 +14151,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -14290,7 +14159,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -14298,7 +14167,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -14306,7 +14175,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -14314,7 +14183,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -14322,7 +14191,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -14330,7 +14199,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -14338,7 +14207,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -14346,7 +14215,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -14354,7 +14223,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -14362,7 +14231,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -14370,7 +14239,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -14378,7 +14247,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -14386,7 +14255,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -14394,7 +14263,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -14402,7 +14271,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -14424,12 +14293,12 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -14437,7 +14306,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -14445,7 +14314,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -14453,7 +14322,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -14461,7 +14330,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -14469,7 +14338,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -14477,7 +14346,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -14485,7 +14354,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -14493,7 +14362,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -14501,7 +14370,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -14509,7 +14378,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -14517,7 +14386,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -14525,7 +14394,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -14533,7 +14402,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -14541,7 +14410,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -14549,7 +14418,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -14557,7 +14426,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -14565,7 +14434,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -14573,7 +14442,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -14581,7 +14450,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -14589,7 +14458,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -14597,7 +14466,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -14605,7 +14474,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -14613,7 +14482,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -14621,7 +14490,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -14629,7 +14498,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -14637,7 +14506,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -14645,7 +14514,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -14653,7 +14522,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -14661,7 +14530,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -14669,7 +14538,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -14677,7 +14546,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -14685,7 +14554,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -14693,7 +14562,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -14701,7 +14570,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -14709,7 +14578,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
@@ -14717,7 +14586,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
@@ -14725,7 +14594,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -14733,7 +14602,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -14741,7 +14610,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -14749,7 +14618,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -14757,7 +14626,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
@@ -14765,7 +14634,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
@@ -14773,7 +14642,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -14781,7 +14650,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
@@ -14789,7 +14658,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
@@ -14797,7 +14666,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
@@ -14805,7 +14674,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
@@ -14813,7 +14682,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -14821,7 +14690,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
@@ -14829,7 +14698,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C88" t="b">
         <v>0</v>
@@ -16797,44 +16666,44 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
         <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -16842,7 +16711,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -16853,13 +16722,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>56</v>
@@ -16867,7 +16736,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
@@ -16876,7 +16745,7 @@
         <v>2009</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7">
         <v>2009</v>
@@ -16884,50 +16753,50 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>2019</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8">
         <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E9" s="13">
+      <c r="D9" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -16935,16 +16804,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B11" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -16952,16 +16821,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B12" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -16969,16 +16838,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>205</v>
-      </c>
-      <c r="B13" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -16986,16 +16855,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -17003,16 +16872,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -17020,16 +16889,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B16" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -17147,7 +17016,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17166,39 +17035,39 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>180</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="b">
@@ -17210,11 +17079,11 @@
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>44</v>
@@ -17228,11 +17097,11 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -17240,11 +17109,11 @@
       <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>44</v>
@@ -17258,10 +17127,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -17269,11 +17138,11 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>44</v>
@@ -17287,10 +17156,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -17299,10 +17168,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H5" s="4">
         <v>100</v>
@@ -17316,7 +17185,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>1</v>
@@ -17327,11 +17196,11 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>44</v>
@@ -17345,7 +17214,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
@@ -17356,11 +17225,11 @@
       <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>44</v>
@@ -17374,7 +17243,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
@@ -17385,11 +17254,11 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>44</v>
@@ -17403,7 +17272,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>1</v>
@@ -17414,11 +17283,11 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>44</v>
@@ -17432,7 +17301,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>1</v>
@@ -17443,11 +17312,11 @@
       <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>44</v>
@@ -17461,7 +17330,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="4" t="b">
         <v>1</v>
@@ -17477,7 +17346,7 @@
         <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H11" s="4">
         <v>100</v>
@@ -17491,7 +17360,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4" t="b">
         <v>1</v>
@@ -17507,7 +17376,7 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H12" s="4">
         <v>100</v>
@@ -17521,7 +17390,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="4" t="b">
         <v>1</v>
@@ -17537,7 +17406,7 @@
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H13" s="4">
         <v>100</v>
@@ -17551,7 +17420,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="4" t="b">
         <v>1</v>
@@ -17567,7 +17436,7 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H14" s="4">
         <v>100</v>
@@ -17581,7 +17450,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="4" t="b">
         <v>1</v>
@@ -17597,7 +17466,7 @@
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H15" s="4">
         <v>100</v>
@@ -17611,7 +17480,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C16" s="4" t="b">
         <v>1</v>
@@ -17623,12 +17492,12 @@
       <c r="E16" s="4">
         <v>-0.23</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <f>100-F11</f>
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H16" s="4">
         <v>0</v>
@@ -17642,7 +17511,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C17" s="4" t="b">
         <v>1</v>
@@ -17654,12 +17523,12 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <f t="shared" ref="F17:F20" si="2">100-F12</f>
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H17" s="4">
         <v>0</v>
@@ -17673,7 +17542,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C18" s="4" t="b">
         <v>1</v>
@@ -17685,12 +17554,12 @@
       <c r="E18" s="4">
         <v>-0.27</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H18" s="4">
         <v>0</v>
@@ -17704,7 +17573,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C19" s="4" t="b">
         <v>1</v>
@@ -17716,12 +17585,12 @@
       <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
@@ -17735,7 +17604,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C20" s="4" t="b">
         <v>1</v>
@@ -17747,12 +17616,12 @@
       <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
@@ -17766,7 +17635,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="4" t="b">
         <v>1</v>
@@ -17777,11 +17646,11 @@
       <c r="E21" s="4">
         <v>0</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>44</v>
@@ -17795,7 +17664,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="4" t="b">
         <v>1</v>
@@ -17806,11 +17675,11 @@
       <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>44</v>
@@ -17824,7 +17693,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="4" t="b">
         <v>1</v>
@@ -17835,11 +17704,11 @@
       <c r="E23" s="4">
         <v>0.33</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>44</v>
@@ -17853,31 +17722,31 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="9"/>
+        <v>181</v>
+      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="6">
         <v>0.7</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>0.7</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="H24" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>44</v>
       </c>
       <c r="I24" s="6">
         <v>0</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>0</v>
       </c>
     </row>
@@ -18419,41 +18288,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>0.45</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2">
         <v>0.45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="11">
         <v>0.83115000000000006</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="12">
+      <c r="C3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="11">
         <v>0.83115000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -18461,13 +18330,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -18475,13 +18344,13 @@
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -18527,72 +18396,72 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -18601,7 +18470,7 @@
         <v>2018</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6">
         <v>2018</v>
@@ -18686,7 +18555,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -18697,32 +18566,32 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>104</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -18731,7 +18600,7 @@
         <v>2019</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5">
         <v>2019</v>
@@ -18739,7 +18608,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -18748,41 +18617,41 @@
         <v>0.5</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="13">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -18863,13 +18732,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modal split instance output and start of historical production volume output
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\OneDrive - TUM\Documents\Master_Semester_1\IDP\endemo2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6329F33F-54D7-4E58-A8CE-A722F9D92EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD457FA2-A1F1-41FA-989E-1B3428789EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1610" yWindow="610" windowWidth="19200" windowHeight="11260" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="2320" windowWidth="19200" windowHeight="11260" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -828,7 +828,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,7 +1028,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1116,7 +1116,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13562,7 +13562,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13617,7 +13617,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
@@ -13631,7 +13631,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
@@ -13659,7 +13659,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
advancements in transport sector
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\OneDrive - TUM\Documents\Master_Semester_1\IDP\endemo2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD457FA2-A1F1-41FA-989E-1B3428789EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB07CD29-AB7E-41C9-AF15-BCF27632C691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2320" windowWidth="19200" windowHeight="11260" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37245" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="730" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -840,11 +840,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
@@ -852,7 +852,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
@@ -928,11 +928,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13561,8 +13561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17015,8 +17015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E5C615-F815-41AB-BEEF-C7C927BFC703}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17071,7 +17071,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -17101,7 +17101,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -17130,7 +17130,7 @@
         <v>163</v>
       </c>
       <c r="C4" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -17159,7 +17159,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -17217,7 +17217,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>

</xml_diff>

<commit_message>
lots of fixes in transport, a fix in industry and energy carrier consumption detail output
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\OneDrive - TUM\Documents\Master_Semester_1\IDP\endemo2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB07CD29-AB7E-41C9-AF15-BCF27632C691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E78D21-6963-4D59-8648-B76A9D541B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37245" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="730" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="0" windowWidth="12790" windowHeight="15380" tabRatio="730" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -683,17 +683,20 @@
     <t>The defined proportion contributes to hydrogen demand. Values from 0 to 1.</t>
   </si>
   <si>
+    <t>If NUTS2 resolution is activated, population forecast has to be active at least for the first calculation.</t>
+  </si>
+  <si>
     <t>Linear time trend</t>
-  </si>
-  <si>
-    <t>If NUTS2 resolution is activated, population forecast has to be active at least for the first calculation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0_i"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,6 +716,17 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -780,8 +794,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -811,8 +828,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="NumberCellStyle" xfId="1" xr:uid="{79ED66F4-65B5-43B8-B88C-8A58B3803A82}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -940,7 +958,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13562,7 +13580,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13603,7 +13621,7 @@
         <v>44</v>
       </c>
       <c r="C2" s="5">
-        <v>2050</v>
+        <v>2018</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13676,7 +13694,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>56</v>
@@ -13977,8 +13995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16672,7 +16690,7 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
         <v>179</v>
@@ -17016,7 +17034,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17168,7 +17186,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>175</v>
@@ -17343,7 +17361,7 @@
         <v>-0.23</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G11" t="s">
         <v>176</v>
@@ -17373,7 +17391,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
         <v>176</v>
@@ -17403,7 +17421,7 @@
         <v>-0.27</v>
       </c>
       <c r="F13">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
         <v>176</v>
@@ -17433,7 +17451,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>176</v>
@@ -17463,7 +17481,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G15" t="s">
         <v>176</v>
@@ -17494,7 +17512,7 @@
       </c>
       <c r="F16" s="9">
         <f>100-F11</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G16" t="s">
         <v>189</v>
@@ -17525,7 +17543,7 @@
       </c>
       <c r="F17" s="9">
         <f t="shared" ref="F17:F20" si="2">100-F12</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
         <v>189</v>
@@ -17556,7 +17574,7 @@
       </c>
       <c r="F18" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
         <v>189</v>
@@ -17587,7 +17605,7 @@
       </c>
       <c r="F19" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
         <v>189</v>
@@ -17618,7 +17636,7 @@
       </c>
       <c r="F20" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G20" t="s">
         <v>189</v>
@@ -18263,7 +18281,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18367,7 +18385,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18527,7 +18545,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18558,10 +18576,10 @@
         <v>68</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
transport sector demand now matches with reference
</commit_message>
<xml_diff>
--- a/input/Set_and_Control_Parameters.xlsx
+++ b/input/Set_and_Control_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\OneDrive - TUM\Documents\Master_Semester_1\IDP\endemo2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E78D21-6963-4D59-8648-B76A9D541B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B55B0B-5C63-4782-AEA3-EA308020AD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="0" windowWidth="12790" windowHeight="15380" tabRatio="730" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="209">
   <si>
     <t>Country</t>
   </si>
@@ -696,7 +696,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0_i"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,11 +716,6 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -796,7 +791,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
@@ -858,11 +853,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
@@ -870,7 +865,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
@@ -946,11 +941,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1046,7 +1041,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1134,7 +1129,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1266,7 +1261,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13579,8 +13574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13621,7 +13616,7 @@
         <v>44</v>
       </c>
       <c r="C2" s="5">
-        <v>2018</v>
+        <v>2050</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13649,7 +13644,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
@@ -13677,7 +13672,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -13719,7 +13714,7 @@
         <v>51</v>
       </c>
       <c r="C9" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -17033,8 +17028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E5C615-F815-41AB-BEEF-C7C927BFC703}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17089,7 +17084,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -17119,7 +17114,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -17148,7 +17143,7 @@
         <v>163</v>
       </c>
       <c r="C4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -17156,8 +17151,8 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>44</v>
+      <c r="F4" s="9">
+        <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>178</v>
@@ -17177,7 +17172,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -17186,7 +17181,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
         <v>175</v>
@@ -17235,7 +17230,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -17361,7 +17356,7 @@
         <v>-0.23</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
         <v>176</v>
@@ -17391,7 +17386,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>176</v>
@@ -17421,7 +17416,7 @@
         <v>-0.27</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
         <v>176</v>
@@ -17451,7 +17446,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
         <v>176</v>
@@ -17481,7 +17476,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
         <v>176</v>
@@ -17512,7 +17507,7 @@
       </c>
       <c r="F16" s="9">
         <f>100-F11</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G16" t="s">
         <v>189</v>
@@ -17543,7 +17538,7 @@
       </c>
       <c r="F17" s="9">
         <f t="shared" ref="F17:F20" si="2">100-F12</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
         <v>189</v>
@@ -17574,7 +17569,7 @@
       </c>
       <c r="F18" s="9">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>189</v>
@@ -17605,7 +17600,7 @@
       </c>
       <c r="F19" s="9">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G19" t="s">
         <v>189</v>
@@ -17636,7 +17631,7 @@
       </c>
       <c r="F20" s="9">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G20" t="s">
         <v>189</v>

</xml_diff>